<commit_message>
initial commit for making login page
</commit_message>
<xml_diff>
--- a/misc/CMSC 128 Requirements Traceability Matrix for SHUFFLE (Eulin).xlsx
+++ b/misc/CMSC 128 Requirements Traceability Matrix for SHUFFLE (Eulin).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\projects\misc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\shuffle\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028EA9A8-120D-4135-998C-5BB47B0F96C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B949B7-B69B-4412-B7DA-473BC30B7377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="12210" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="2295" windowWidth="14715" windowHeight="9810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RTM" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="333">
   <si>
     <t>Requirements Traceability Matrix (Sample Template)</t>
   </si>
@@ -1822,6 +1822,12 @@
   </si>
   <si>
     <t>schema_diagram</t>
+  </si>
+  <si>
+    <t>polished_ui</t>
+  </si>
+  <si>
+    <t>logo for the app and clean user interface</t>
   </si>
 </sst>
 </file>
@@ -2368,62 +2374,12 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2450,12 +2406,62 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2674,8 +2680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AT1019"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC7" zoomScale="58" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AN26" sqref="AN26"/>
+    <sheetView tabSelected="1" topLeftCell="Y9" zoomScale="71" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AM20" sqref="AM20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2766,10 +2772,10 @@
       <c r="A3" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="C3" s="74"/>
+      <c r="C3" s="52"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -2794,24 +2800,24 @@
       <c r="A4" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="51" t="s">
         <v>129</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="73"/>
-      <c r="N4" s="73"/>
-      <c r="O4" s="73"/>
-      <c r="P4" s="73"/>
-      <c r="Q4" s="73"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="51"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="51"/>
+      <c r="Q4" s="51"/>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
@@ -2822,11 +2828,11 @@
       <c r="A5" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B5" s="75" t="s">
+      <c r="B5" s="53" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -2850,12 +2856,12 @@
       <c r="A6" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B6" s="80" t="s">
+      <c r="B6" s="58" t="s">
         <v>125</v>
       </c>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -2902,13 +2908,13 @@
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="78" t="s">
+      <c r="B7" s="56" t="s">
         <v>126</v>
       </c>
-      <c r="C7" s="79"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="79"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -2956,15 +2962,15 @@
         <v>4</v>
       </c>
       <c r="C8" s="6"/>
-      <c r="D8" s="76" t="s">
+      <c r="D8" s="54" t="s">
         <v>128</v>
       </c>
-      <c r="E8" s="76"/>
-      <c r="F8" s="76"/>
-      <c r="G8" s="76"/>
-      <c r="H8" s="76"/>
-      <c r="I8" s="76"/>
-      <c r="J8" s="76"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -3008,15 +3014,15 @@
         <v>6</v>
       </c>
       <c r="C9" s="6"/>
-      <c r="D9" s="77" t="s">
+      <c r="D9" s="55" t="s">
         <v>127</v>
       </c>
-      <c r="E9" s="76"/>
-      <c r="F9" s="76"/>
-      <c r="G9" s="76"/>
-      <c r="H9" s="76"/>
-      <c r="I9" s="76"/>
-      <c r="J9" s="76"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -3299,57 +3305,57 @@
       <c r="AT14" s="9"/>
     </row>
     <row r="15" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="68" t="s">
+      <c r="B15" s="69"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="59"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="59"/>
-      <c r="N15" s="59"/>
-      <c r="O15" s="59"/>
-      <c r="P15" s="59"/>
-      <c r="Q15" s="59"/>
-      <c r="R15" s="59"/>
-      <c r="S15" s="59"/>
-      <c r="T15" s="59"/>
-      <c r="U15" s="59"/>
-      <c r="V15" s="48"/>
-      <c r="W15" s="69" t="s">
+      <c r="H15" s="69"/>
+      <c r="I15" s="69"/>
+      <c r="J15" s="69"/>
+      <c r="K15" s="69"/>
+      <c r="L15" s="69"/>
+      <c r="M15" s="69"/>
+      <c r="N15" s="69"/>
+      <c r="O15" s="69"/>
+      <c r="P15" s="69"/>
+      <c r="Q15" s="69"/>
+      <c r="R15" s="69"/>
+      <c r="S15" s="69"/>
+      <c r="T15" s="69"/>
+      <c r="U15" s="69"/>
+      <c r="V15" s="60"/>
+      <c r="W15" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="X15" s="59"/>
-      <c r="Y15" s="59"/>
-      <c r="Z15" s="59"/>
-      <c r="AA15" s="59"/>
-      <c r="AB15" s="59"/>
-      <c r="AC15" s="59"/>
-      <c r="AD15" s="59"/>
-      <c r="AE15" s="48"/>
-      <c r="AF15" s="70" t="s">
+      <c r="X15" s="69"/>
+      <c r="Y15" s="69"/>
+      <c r="Z15" s="69"/>
+      <c r="AA15" s="69"/>
+      <c r="AB15" s="69"/>
+      <c r="AC15" s="69"/>
+      <c r="AD15" s="69"/>
+      <c r="AE15" s="60"/>
+      <c r="AF15" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="AG15" s="59"/>
-      <c r="AH15" s="59"/>
-      <c r="AI15" s="59"/>
-      <c r="AJ15" s="59"/>
-      <c r="AK15" s="59"/>
-      <c r="AL15" s="59"/>
-      <c r="AM15" s="48"/>
-      <c r="AN15" s="47" t="s">
+      <c r="AG15" s="69"/>
+      <c r="AH15" s="69"/>
+      <c r="AI15" s="69"/>
+      <c r="AJ15" s="69"/>
+      <c r="AK15" s="69"/>
+      <c r="AL15" s="69"/>
+      <c r="AM15" s="60"/>
+      <c r="AN15" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="AO15" s="48"/>
+      <c r="AO15" s="60"/>
       <c r="AP15" s="10"/>
       <c r="AQ15" s="10"/>
       <c r="AR15" s="10"/>
@@ -3357,47 +3363,47 @@
       <c r="AT15" s="10"/>
     </row>
     <row r="16" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="49"/>
-      <c r="B16" s="60"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="60"/>
-      <c r="J16" s="60"/>
-      <c r="K16" s="60"/>
-      <c r="L16" s="60"/>
-      <c r="M16" s="60"/>
-      <c r="N16" s="60"/>
-      <c r="O16" s="60"/>
-      <c r="P16" s="60"/>
-      <c r="Q16" s="60"/>
-      <c r="R16" s="60"/>
-      <c r="S16" s="60"/>
-      <c r="T16" s="60"/>
-      <c r="U16" s="60"/>
-      <c r="V16" s="50"/>
-      <c r="W16" s="51"/>
-      <c r="X16" s="61"/>
-      <c r="Y16" s="61"/>
-      <c r="Z16" s="61"/>
-      <c r="AA16" s="61"/>
-      <c r="AB16" s="61"/>
-      <c r="AC16" s="61"/>
-      <c r="AD16" s="61"/>
-      <c r="AE16" s="52"/>
-      <c r="AF16" s="49"/>
-      <c r="AG16" s="60"/>
-      <c r="AH16" s="60"/>
-      <c r="AI16" s="60"/>
-      <c r="AJ16" s="60"/>
-      <c r="AK16" s="60"/>
-      <c r="AL16" s="60"/>
-      <c r="AM16" s="50"/>
-      <c r="AN16" s="49"/>
-      <c r="AO16" s="50"/>
+      <c r="A16" s="61"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="70"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="70"/>
+      <c r="I16" s="70"/>
+      <c r="J16" s="70"/>
+      <c r="K16" s="70"/>
+      <c r="L16" s="70"/>
+      <c r="M16" s="70"/>
+      <c r="N16" s="70"/>
+      <c r="O16" s="70"/>
+      <c r="P16" s="70"/>
+      <c r="Q16" s="70"/>
+      <c r="R16" s="70"/>
+      <c r="S16" s="70"/>
+      <c r="T16" s="70"/>
+      <c r="U16" s="70"/>
+      <c r="V16" s="62"/>
+      <c r="W16" s="63"/>
+      <c r="X16" s="71"/>
+      <c r="Y16" s="71"/>
+      <c r="Z16" s="71"/>
+      <c r="AA16" s="71"/>
+      <c r="AB16" s="71"/>
+      <c r="AC16" s="71"/>
+      <c r="AD16" s="71"/>
+      <c r="AE16" s="64"/>
+      <c r="AF16" s="61"/>
+      <c r="AG16" s="70"/>
+      <c r="AH16" s="70"/>
+      <c r="AI16" s="70"/>
+      <c r="AJ16" s="70"/>
+      <c r="AK16" s="70"/>
+      <c r="AL16" s="70"/>
+      <c r="AM16" s="62"/>
+      <c r="AN16" s="61"/>
+      <c r="AO16" s="62"/>
       <c r="AP16" s="10"/>
       <c r="AQ16" s="10"/>
       <c r="AR16" s="10"/>
@@ -3405,53 +3411,53 @@
       <c r="AT16" s="10"/>
     </row>
     <row r="17" spans="1:46" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="51"/>
-      <c r="B17" s="61"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="61"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="61"/>
-      <c r="L17" s="61"/>
-      <c r="M17" s="61"/>
-      <c r="N17" s="61"/>
-      <c r="O17" s="61"/>
-      <c r="P17" s="61"/>
-      <c r="Q17" s="61"/>
-      <c r="R17" s="61"/>
-      <c r="S17" s="61"/>
-      <c r="T17" s="61"/>
-      <c r="U17" s="61"/>
-      <c r="V17" s="52"/>
-      <c r="W17" s="53" t="s">
+      <c r="A17" s="63"/>
+      <c r="B17" s="71"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="71"/>
+      <c r="J17" s="71"/>
+      <c r="K17" s="71"/>
+      <c r="L17" s="71"/>
+      <c r="M17" s="71"/>
+      <c r="N17" s="71"/>
+      <c r="O17" s="71"/>
+      <c r="P17" s="71"/>
+      <c r="Q17" s="71"/>
+      <c r="R17" s="71"/>
+      <c r="S17" s="71"/>
+      <c r="T17" s="71"/>
+      <c r="U17" s="71"/>
+      <c r="V17" s="64"/>
+      <c r="W17" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="X17" s="54"/>
-      <c r="Y17" s="55"/>
-      <c r="Z17" s="56" t="s">
+      <c r="X17" s="48"/>
+      <c r="Y17" s="49"/>
+      <c r="Z17" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="AA17" s="54"/>
-      <c r="AB17" s="55"/>
-      <c r="AC17" s="57" t="s">
+      <c r="AA17" s="48"/>
+      <c r="AB17" s="49"/>
+      <c r="AC17" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="AD17" s="54"/>
-      <c r="AE17" s="55"/>
-      <c r="AF17" s="51"/>
-      <c r="AG17" s="61"/>
-      <c r="AH17" s="61"/>
-      <c r="AI17" s="61"/>
-      <c r="AJ17" s="61"/>
-      <c r="AK17" s="61"/>
-      <c r="AL17" s="61"/>
-      <c r="AM17" s="52"/>
-      <c r="AN17" s="49"/>
-      <c r="AO17" s="50"/>
+      <c r="AD17" s="48"/>
+      <c r="AE17" s="49"/>
+      <c r="AF17" s="63"/>
+      <c r="AG17" s="71"/>
+      <c r="AH17" s="71"/>
+      <c r="AI17" s="71"/>
+      <c r="AJ17" s="71"/>
+      <c r="AK17" s="71"/>
+      <c r="AL17" s="71"/>
+      <c r="AM17" s="64"/>
+      <c r="AN17" s="61"/>
+      <c r="AO17" s="62"/>
       <c r="AP17" s="10"/>
       <c r="AQ17" s="10"/>
       <c r="AR17" s="10"/>
@@ -3459,69 +3465,69 @@
       <c r="AT17" s="10"/>
     </row>
     <row r="18" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A18" s="62" t="s">
+      <c r="A18" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="54"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="63" t="s">
+      <c r="B18" s="48"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="64" t="s">
+      <c r="H18" s="48"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="L18" s="54"/>
-      <c r="M18" s="54"/>
-      <c r="N18" s="55"/>
-      <c r="O18" s="65" t="s">
+      <c r="L18" s="48"/>
+      <c r="M18" s="48"/>
+      <c r="N18" s="49"/>
+      <c r="O18" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="P18" s="54"/>
-      <c r="Q18" s="55"/>
-      <c r="R18" s="71" t="s">
+      <c r="P18" s="48"/>
+      <c r="Q18" s="49"/>
+      <c r="R18" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="S18" s="54"/>
-      <c r="T18" s="54"/>
-      <c r="U18" s="54"/>
-      <c r="V18" s="55"/>
-      <c r="W18" s="72" t="s">
+      <c r="S18" s="48"/>
+      <c r="T18" s="48"/>
+      <c r="U18" s="48"/>
+      <c r="V18" s="49"/>
+      <c r="W18" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="X18" s="54"/>
-      <c r="Y18" s="55"/>
-      <c r="Z18" s="72" t="s">
+      <c r="X18" s="48"/>
+      <c r="Y18" s="49"/>
+      <c r="Z18" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="AA18" s="54"/>
-      <c r="AB18" s="55"/>
-      <c r="AC18" s="72" t="s">
+      <c r="AA18" s="48"/>
+      <c r="AB18" s="49"/>
+      <c r="AC18" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="AD18" s="54"/>
-      <c r="AE18" s="55"/>
-      <c r="AF18" s="66" t="s">
+      <c r="AD18" s="48"/>
+      <c r="AE18" s="49"/>
+      <c r="AF18" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="AG18" s="54"/>
-      <c r="AH18" s="55"/>
-      <c r="AI18" s="66" t="s">
+      <c r="AG18" s="48"/>
+      <c r="AH18" s="49"/>
+      <c r="AI18" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="AJ18" s="54"/>
-      <c r="AK18" s="55"/>
-      <c r="AL18" s="67" t="s">
+      <c r="AJ18" s="48"/>
+      <c r="AK18" s="49"/>
+      <c r="AL18" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="AM18" s="52"/>
-      <c r="AN18" s="51"/>
-      <c r="AO18" s="52"/>
+      <c r="AM18" s="64"/>
+      <c r="AN18" s="63"/>
+      <c r="AO18" s="64"/>
       <c r="AP18" s="10"/>
       <c r="AQ18" s="10"/>
       <c r="AR18" s="10"/>
@@ -3758,12 +3764,12 @@
         <v>306</v>
       </c>
       <c r="AK20" s="18" t="s">
-        <v>106</v>
+        <v>298</v>
       </c>
       <c r="AL20" s="17" t="s">
         <v>330</v>
       </c>
-      <c r="AM20" s="15" t="s">
+      <c r="AM20" s="30" t="s">
         <v>329</v>
       </c>
       <c r="AN20" s="17" t="s">
@@ -4813,8 +4819,12 @@
       <c r="AF32" s="20"/>
       <c r="AG32" s="20"/>
       <c r="AH32" s="20"/>
-      <c r="AI32" s="20"/>
-      <c r="AJ32" s="20"/>
+      <c r="AI32" s="20" t="s">
+        <v>331</v>
+      </c>
+      <c r="AJ32" s="20" t="s">
+        <v>332</v>
+      </c>
       <c r="AK32" s="20"/>
       <c r="AL32" s="20"/>
       <c r="AM32" s="20"/>
@@ -16793,16 +16803,6 @@
     <row r="1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="Z18:AB18"/>
-    <mergeCell ref="AC18:AE18"/>
-    <mergeCell ref="AF18:AH18"/>
-    <mergeCell ref="B4:Q4"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="D8:J8"/>
-    <mergeCell ref="D9:J9"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B6:E6"/>
     <mergeCell ref="AN15:AO18"/>
     <mergeCell ref="W17:Y17"/>
     <mergeCell ref="Z17:AB17"/>
@@ -16819,6 +16819,16 @@
     <mergeCell ref="AF15:AM17"/>
     <mergeCell ref="R18:V18"/>
     <mergeCell ref="W18:Y18"/>
+    <mergeCell ref="Z18:AB18"/>
+    <mergeCell ref="AC18:AE18"/>
+    <mergeCell ref="AF18:AH18"/>
+    <mergeCell ref="B4:Q4"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="D8:J8"/>
+    <mergeCell ref="D9:J9"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B6:E6"/>
   </mergeCells>
   <phoneticPr fontId="21" type="noConversion"/>
   <hyperlinks>
@@ -16830,6 +16840,7 @@
     <hyperlink ref="AA21" r:id="rId6" xr:uid="{1F1D9C93-0B62-4141-9155-0BF56B97D418}"/>
     <hyperlink ref="AD20" r:id="rId7" xr:uid="{11979102-4C6A-4DD8-920A-409D640D74E1}"/>
     <hyperlink ref="AG20" r:id="rId8" xr:uid="{F3612EEF-6515-43FA-9410-0BDE97984233}"/>
+    <hyperlink ref="AM20" r:id="rId9" xr:uid="{1C6FF353-7903-4FB1-B22F-D98D8E8CD6DD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -16952,17 +16963,17 @@
       <c r="V3" s="2"/>
     </row>
     <row r="4" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="84" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
@@ -17452,57 +17463,57 @@
       <c r="AT14" s="9"/>
     </row>
     <row r="15" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="68" t="s">
+      <c r="B15" s="69"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="59"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="59"/>
-      <c r="N15" s="59"/>
-      <c r="O15" s="59"/>
-      <c r="P15" s="59"/>
-      <c r="Q15" s="59"/>
-      <c r="R15" s="59"/>
-      <c r="S15" s="59"/>
-      <c r="T15" s="59"/>
-      <c r="U15" s="59"/>
-      <c r="V15" s="48"/>
-      <c r="W15" s="69" t="s">
+      <c r="H15" s="69"/>
+      <c r="I15" s="69"/>
+      <c r="J15" s="69"/>
+      <c r="K15" s="69"/>
+      <c r="L15" s="69"/>
+      <c r="M15" s="69"/>
+      <c r="N15" s="69"/>
+      <c r="O15" s="69"/>
+      <c r="P15" s="69"/>
+      <c r="Q15" s="69"/>
+      <c r="R15" s="69"/>
+      <c r="S15" s="69"/>
+      <c r="T15" s="69"/>
+      <c r="U15" s="69"/>
+      <c r="V15" s="60"/>
+      <c r="W15" s="78" t="s">
         <v>78</v>
       </c>
-      <c r="X15" s="59"/>
-      <c r="Y15" s="59"/>
-      <c r="Z15" s="59"/>
-      <c r="AA15" s="59"/>
-      <c r="AB15" s="59"/>
-      <c r="AC15" s="59"/>
-      <c r="AD15" s="59"/>
-      <c r="AE15" s="48"/>
-      <c r="AF15" s="70" t="s">
+      <c r="X15" s="69"/>
+      <c r="Y15" s="69"/>
+      <c r="Z15" s="69"/>
+      <c r="AA15" s="69"/>
+      <c r="AB15" s="69"/>
+      <c r="AC15" s="69"/>
+      <c r="AD15" s="69"/>
+      <c r="AE15" s="60"/>
+      <c r="AF15" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="AG15" s="59"/>
-      <c r="AH15" s="59"/>
-      <c r="AI15" s="59"/>
-      <c r="AJ15" s="59"/>
-      <c r="AK15" s="59"/>
-      <c r="AL15" s="59"/>
-      <c r="AM15" s="48"/>
-      <c r="AN15" s="47" t="s">
+      <c r="AG15" s="69"/>
+      <c r="AH15" s="69"/>
+      <c r="AI15" s="69"/>
+      <c r="AJ15" s="69"/>
+      <c r="AK15" s="69"/>
+      <c r="AL15" s="69"/>
+      <c r="AM15" s="60"/>
+      <c r="AN15" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="AO15" s="48"/>
+      <c r="AO15" s="60"/>
       <c r="AP15" s="10"/>
       <c r="AQ15" s="10"/>
       <c r="AR15" s="10"/>
@@ -17510,47 +17521,47 @@
       <c r="AT15" s="10"/>
     </row>
     <row r="16" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="49"/>
-      <c r="B16" s="60"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="60"/>
-      <c r="J16" s="60"/>
-      <c r="K16" s="60"/>
-      <c r="L16" s="60"/>
-      <c r="M16" s="60"/>
-      <c r="N16" s="60"/>
-      <c r="O16" s="60"/>
-      <c r="P16" s="60"/>
-      <c r="Q16" s="60"/>
-      <c r="R16" s="60"/>
-      <c r="S16" s="60"/>
-      <c r="T16" s="60"/>
-      <c r="U16" s="60"/>
-      <c r="V16" s="50"/>
-      <c r="W16" s="51"/>
-      <c r="X16" s="61"/>
-      <c r="Y16" s="61"/>
-      <c r="Z16" s="61"/>
-      <c r="AA16" s="61"/>
-      <c r="AB16" s="61"/>
-      <c r="AC16" s="61"/>
-      <c r="AD16" s="61"/>
-      <c r="AE16" s="52"/>
-      <c r="AF16" s="49"/>
-      <c r="AG16" s="60"/>
-      <c r="AH16" s="60"/>
-      <c r="AI16" s="60"/>
-      <c r="AJ16" s="60"/>
-      <c r="AK16" s="60"/>
-      <c r="AL16" s="60"/>
-      <c r="AM16" s="50"/>
-      <c r="AN16" s="49"/>
-      <c r="AO16" s="50"/>
+      <c r="A16" s="61"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="70"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="70"/>
+      <c r="I16" s="70"/>
+      <c r="J16" s="70"/>
+      <c r="K16" s="70"/>
+      <c r="L16" s="70"/>
+      <c r="M16" s="70"/>
+      <c r="N16" s="70"/>
+      <c r="O16" s="70"/>
+      <c r="P16" s="70"/>
+      <c r="Q16" s="70"/>
+      <c r="R16" s="70"/>
+      <c r="S16" s="70"/>
+      <c r="T16" s="70"/>
+      <c r="U16" s="70"/>
+      <c r="V16" s="62"/>
+      <c r="W16" s="63"/>
+      <c r="X16" s="71"/>
+      <c r="Y16" s="71"/>
+      <c r="Z16" s="71"/>
+      <c r="AA16" s="71"/>
+      <c r="AB16" s="71"/>
+      <c r="AC16" s="71"/>
+      <c r="AD16" s="71"/>
+      <c r="AE16" s="64"/>
+      <c r="AF16" s="61"/>
+      <c r="AG16" s="70"/>
+      <c r="AH16" s="70"/>
+      <c r="AI16" s="70"/>
+      <c r="AJ16" s="70"/>
+      <c r="AK16" s="70"/>
+      <c r="AL16" s="70"/>
+      <c r="AM16" s="62"/>
+      <c r="AN16" s="61"/>
+      <c r="AO16" s="62"/>
       <c r="AP16" s="10"/>
       <c r="AQ16" s="10"/>
       <c r="AR16" s="10"/>
@@ -17558,53 +17569,53 @@
       <c r="AT16" s="10"/>
     </row>
     <row r="17" spans="1:46" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="51"/>
-      <c r="B17" s="61"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="61"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="61"/>
-      <c r="L17" s="61"/>
-      <c r="M17" s="61"/>
-      <c r="N17" s="61"/>
-      <c r="O17" s="61"/>
-      <c r="P17" s="61"/>
-      <c r="Q17" s="61"/>
-      <c r="R17" s="61"/>
-      <c r="S17" s="61"/>
-      <c r="T17" s="61"/>
-      <c r="U17" s="61"/>
-      <c r="V17" s="52"/>
-      <c r="W17" s="53" t="s">
+      <c r="A17" s="63"/>
+      <c r="B17" s="71"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="71"/>
+      <c r="J17" s="71"/>
+      <c r="K17" s="71"/>
+      <c r="L17" s="71"/>
+      <c r="M17" s="71"/>
+      <c r="N17" s="71"/>
+      <c r="O17" s="71"/>
+      <c r="P17" s="71"/>
+      <c r="Q17" s="71"/>
+      <c r="R17" s="71"/>
+      <c r="S17" s="71"/>
+      <c r="T17" s="71"/>
+      <c r="U17" s="71"/>
+      <c r="V17" s="64"/>
+      <c r="W17" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="X17" s="54"/>
-      <c r="Y17" s="55"/>
-      <c r="Z17" s="56" t="s">
+      <c r="X17" s="48"/>
+      <c r="Y17" s="49"/>
+      <c r="Z17" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="AA17" s="54"/>
-      <c r="AB17" s="55"/>
-      <c r="AC17" s="57" t="s">
+      <c r="AA17" s="48"/>
+      <c r="AB17" s="49"/>
+      <c r="AC17" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="AD17" s="54"/>
-      <c r="AE17" s="55"/>
-      <c r="AF17" s="51"/>
-      <c r="AG17" s="61"/>
-      <c r="AH17" s="61"/>
-      <c r="AI17" s="61"/>
-      <c r="AJ17" s="61"/>
-      <c r="AK17" s="61"/>
-      <c r="AL17" s="61"/>
-      <c r="AM17" s="52"/>
-      <c r="AN17" s="49"/>
-      <c r="AO17" s="50"/>
+      <c r="AD17" s="48"/>
+      <c r="AE17" s="49"/>
+      <c r="AF17" s="63"/>
+      <c r="AG17" s="71"/>
+      <c r="AH17" s="71"/>
+      <c r="AI17" s="71"/>
+      <c r="AJ17" s="71"/>
+      <c r="AK17" s="71"/>
+      <c r="AL17" s="71"/>
+      <c r="AM17" s="64"/>
+      <c r="AN17" s="61"/>
+      <c r="AO17" s="62"/>
       <c r="AP17" s="10"/>
       <c r="AQ17" s="10"/>
       <c r="AR17" s="10"/>
@@ -17612,69 +17623,69 @@
       <c r="AT17" s="10"/>
     </row>
     <row r="18" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A18" s="62" t="s">
+      <c r="A18" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="54"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="63" t="s">
+      <c r="B18" s="48"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="64" t="s">
+      <c r="H18" s="48"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="L18" s="54"/>
-      <c r="M18" s="54"/>
-      <c r="N18" s="55"/>
-      <c r="O18" s="65" t="s">
+      <c r="L18" s="48"/>
+      <c r="M18" s="48"/>
+      <c r="N18" s="49"/>
+      <c r="O18" s="75" t="s">
         <v>80</v>
       </c>
-      <c r="P18" s="54"/>
-      <c r="Q18" s="55"/>
-      <c r="R18" s="71" t="s">
+      <c r="P18" s="48"/>
+      <c r="Q18" s="49"/>
+      <c r="R18" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="S18" s="54"/>
-      <c r="T18" s="54"/>
-      <c r="U18" s="54"/>
-      <c r="V18" s="55"/>
-      <c r="W18" s="72" t="s">
+      <c r="S18" s="48"/>
+      <c r="T18" s="48"/>
+      <c r="U18" s="48"/>
+      <c r="V18" s="49"/>
+      <c r="W18" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="X18" s="54"/>
-      <c r="Y18" s="55"/>
-      <c r="Z18" s="72" t="s">
+      <c r="X18" s="48"/>
+      <c r="Y18" s="49"/>
+      <c r="Z18" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="AA18" s="54"/>
-      <c r="AB18" s="55"/>
-      <c r="AC18" s="72" t="s">
+      <c r="AA18" s="48"/>
+      <c r="AB18" s="49"/>
+      <c r="AC18" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="AD18" s="54"/>
-      <c r="AE18" s="55"/>
-      <c r="AF18" s="66" t="s">
+      <c r="AD18" s="48"/>
+      <c r="AE18" s="49"/>
+      <c r="AF18" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="AG18" s="54"/>
-      <c r="AH18" s="55"/>
-      <c r="AI18" s="66" t="s">
+      <c r="AG18" s="48"/>
+      <c r="AH18" s="49"/>
+      <c r="AI18" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="AJ18" s="54"/>
-      <c r="AK18" s="55"/>
-      <c r="AL18" s="67" t="s">
+      <c r="AJ18" s="48"/>
+      <c r="AK18" s="49"/>
+      <c r="AL18" s="76" t="s">
         <v>85</v>
       </c>
-      <c r="AM18" s="52"/>
-      <c r="AN18" s="51"/>
-      <c r="AO18" s="52"/>
+      <c r="AM18" s="64"/>
+      <c r="AN18" s="63"/>
+      <c r="AO18" s="64"/>
       <c r="AP18" s="10"/>
       <c r="AQ18" s="10"/>
       <c r="AR18" s="10"/>
@@ -17900,55 +17911,55 @@
       <c r="AT20" s="19"/>
     </row>
     <row r="21" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="82" t="s">
+      <c r="A21" s="81" t="s">
         <v>93</v>
       </c>
-      <c r="B21" s="82" t="s">
+      <c r="B21" s="81" t="s">
         <v>94</v>
       </c>
-      <c r="C21" s="82" t="s">
+      <c r="C21" s="81" t="s">
         <v>95</v>
       </c>
-      <c r="D21" s="82" t="s">
+      <c r="D21" s="81" t="s">
         <v>96</v>
       </c>
-      <c r="E21" s="85">
+      <c r="E21" s="86">
         <v>44650</v>
       </c>
-      <c r="F21" s="82">
+      <c r="F21" s="81">
         <v>1</v>
       </c>
-      <c r="G21" s="82" t="s">
+      <c r="G21" s="81" t="s">
         <v>97</v>
       </c>
-      <c r="H21" s="82" t="s">
+      <c r="H21" s="81" t="s">
         <v>98</v>
       </c>
-      <c r="I21" s="82" t="s">
+      <c r="I21" s="81" t="s">
         <v>99</v>
       </c>
-      <c r="J21" s="82">
+      <c r="J21" s="81">
         <v>1</v>
       </c>
-      <c r="K21" s="86" t="s">
+      <c r="K21" s="83" t="s">
         <v>100</v>
       </c>
-      <c r="L21" s="82" t="s">
+      <c r="L21" s="81" t="s">
         <v>101</v>
       </c>
-      <c r="M21" s="82" t="s">
+      <c r="M21" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="N21" s="82" t="s">
+      <c r="N21" s="81" t="s">
         <v>103</v>
       </c>
-      <c r="O21" s="82" t="s">
+      <c r="O21" s="81" t="s">
         <v>104</v>
       </c>
-      <c r="P21" s="82" t="s">
+      <c r="P21" s="81" t="s">
         <v>105</v>
       </c>
-      <c r="Q21" s="82" t="s">
+      <c r="Q21" s="81" t="s">
         <v>106</v>
       </c>
       <c r="R21" s="20" t="s">
@@ -17994,23 +18005,23 @@
       <c r="AT21" s="2"/>
     </row>
     <row r="22" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="84"/>
-      <c r="B22" s="84"/>
-      <c r="C22" s="84"/>
-      <c r="D22" s="84"/>
-      <c r="E22" s="84"/>
-      <c r="F22" s="84"/>
-      <c r="G22" s="83"/>
-      <c r="H22" s="83"/>
-      <c r="I22" s="83"/>
-      <c r="J22" s="83"/>
-      <c r="K22" s="52"/>
-      <c r="L22" s="83"/>
-      <c r="M22" s="83"/>
-      <c r="N22" s="83"/>
-      <c r="O22" s="83"/>
-      <c r="P22" s="83"/>
-      <c r="Q22" s="83"/>
+      <c r="A22" s="85"/>
+      <c r="B22" s="85"/>
+      <c r="C22" s="85"/>
+      <c r="D22" s="85"/>
+      <c r="E22" s="85"/>
+      <c r="F22" s="85"/>
+      <c r="G22" s="82"/>
+      <c r="H22" s="82"/>
+      <c r="I22" s="82"/>
+      <c r="J22" s="82"/>
+      <c r="K22" s="64"/>
+      <c r="L22" s="82"/>
+      <c r="M22" s="82"/>
+      <c r="N22" s="82"/>
+      <c r="O22" s="82"/>
+      <c r="P22" s="82"/>
+      <c r="Q22" s="82"/>
       <c r="R22" s="20" t="s">
         <v>113</v>
       </c>
@@ -18044,12 +18055,12 @@
       <c r="AT22" s="2"/>
     </row>
     <row r="23" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="84"/>
-      <c r="B23" s="84"/>
-      <c r="C23" s="84"/>
-      <c r="D23" s="84"/>
-      <c r="E23" s="84"/>
-      <c r="F23" s="84"/>
+      <c r="A23" s="85"/>
+      <c r="B23" s="85"/>
+      <c r="C23" s="85"/>
+      <c r="D23" s="85"/>
+      <c r="E23" s="85"/>
+      <c r="F23" s="85"/>
       <c r="G23" s="20" t="s">
         <v>114</v>
       </c>
@@ -18100,12 +18111,12 @@
       <c r="AT23" s="2"/>
     </row>
     <row r="24" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="83"/>
-      <c r="B24" s="83"/>
-      <c r="C24" s="83"/>
-      <c r="D24" s="83"/>
-      <c r="E24" s="83"/>
-      <c r="F24" s="83"/>
+      <c r="A24" s="82"/>
+      <c r="B24" s="82"/>
+      <c r="C24" s="82"/>
+      <c r="D24" s="82"/>
+      <c r="E24" s="82"/>
+      <c r="F24" s="82"/>
       <c r="G24" s="20" t="s">
         <v>117</v>
       </c>
@@ -29353,15 +29364,22 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="P21:P22"/>
-    <mergeCell ref="Q21:Q22"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="L21:L22"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="N21:N22"/>
-    <mergeCell ref="O21:O22"/>
+    <mergeCell ref="AF15:AM17"/>
+    <mergeCell ref="AN15:AO18"/>
+    <mergeCell ref="W17:Y17"/>
+    <mergeCell ref="Z17:AB17"/>
+    <mergeCell ref="AC17:AE17"/>
+    <mergeCell ref="W18:Y18"/>
+    <mergeCell ref="Z18:AB18"/>
+    <mergeCell ref="AC18:AE18"/>
+    <mergeCell ref="AF18:AH18"/>
+    <mergeCell ref="AI18:AK18"/>
+    <mergeCell ref="AL18:AM18"/>
+    <mergeCell ref="K18:N18"/>
+    <mergeCell ref="O18:Q18"/>
+    <mergeCell ref="R18:V18"/>
+    <mergeCell ref="G15:V17"/>
+    <mergeCell ref="W15:AE16"/>
     <mergeCell ref="A4:I4"/>
     <mergeCell ref="G21:G22"/>
     <mergeCell ref="H21:H22"/>
@@ -29374,22 +29392,15 @@
     <mergeCell ref="A21:A24"/>
     <mergeCell ref="A15:F17"/>
     <mergeCell ref="A18:F18"/>
-    <mergeCell ref="K18:N18"/>
-    <mergeCell ref="O18:Q18"/>
-    <mergeCell ref="R18:V18"/>
-    <mergeCell ref="G15:V17"/>
-    <mergeCell ref="W15:AE16"/>
-    <mergeCell ref="AF15:AM17"/>
-    <mergeCell ref="AN15:AO18"/>
-    <mergeCell ref="W17:Y17"/>
-    <mergeCell ref="Z17:AB17"/>
-    <mergeCell ref="AC17:AE17"/>
-    <mergeCell ref="W18:Y18"/>
-    <mergeCell ref="Z18:AB18"/>
-    <mergeCell ref="AC18:AE18"/>
-    <mergeCell ref="AF18:AH18"/>
-    <mergeCell ref="AI18:AK18"/>
-    <mergeCell ref="AL18:AM18"/>
+    <mergeCell ref="P21:P22"/>
+    <mergeCell ref="Q21:Q22"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="N21:N22"/>
+    <mergeCell ref="O21:O22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
initial commit to login page branch
</commit_message>
<xml_diff>
--- a/misc/CMSC 128 Requirements Traceability Matrix for SHUFFLE (Eulin).xlsx
+++ b/misc/CMSC 128 Requirements Traceability Matrix for SHUFFLE (Eulin).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\projects\misc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\shuffle\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028EA9A8-120D-4135-998C-5BB47B0F96C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B949B7-B69B-4412-B7DA-473BC30B7377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="12210" windowHeight="13605" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="2295" windowWidth="14715" windowHeight="9810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RTM" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="333">
   <si>
     <t>Requirements Traceability Matrix (Sample Template)</t>
   </si>
@@ -1822,6 +1822,12 @@
   </si>
   <si>
     <t>schema_diagram</t>
+  </si>
+  <si>
+    <t>polished_ui</t>
+  </si>
+  <si>
+    <t>logo for the app and clean user interface</t>
   </si>
 </sst>
 </file>
@@ -2368,62 +2374,12 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2450,12 +2406,62 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2674,8 +2680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AT1019"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC7" zoomScale="58" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AN26" sqref="AN26"/>
+    <sheetView tabSelected="1" topLeftCell="Y9" zoomScale="71" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AM20" sqref="AM20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2766,10 +2772,10 @@
       <c r="A3" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="C3" s="74"/>
+      <c r="C3" s="52"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -2794,24 +2800,24 @@
       <c r="A4" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="51" t="s">
         <v>129</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="73"/>
-      <c r="N4" s="73"/>
-      <c r="O4" s="73"/>
-      <c r="P4" s="73"/>
-      <c r="Q4" s="73"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="51"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="51"/>
+      <c r="Q4" s="51"/>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
@@ -2822,11 +2828,11 @@
       <c r="A5" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B5" s="75" t="s">
+      <c r="B5" s="53" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -2850,12 +2856,12 @@
       <c r="A6" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B6" s="80" t="s">
+      <c r="B6" s="58" t="s">
         <v>125</v>
       </c>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -2902,13 +2908,13 @@
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="78" t="s">
+      <c r="B7" s="56" t="s">
         <v>126</v>
       </c>
-      <c r="C7" s="79"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="79"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -2956,15 +2962,15 @@
         <v>4</v>
       </c>
       <c r="C8" s="6"/>
-      <c r="D8" s="76" t="s">
+      <c r="D8" s="54" t="s">
         <v>128</v>
       </c>
-      <c r="E8" s="76"/>
-      <c r="F8" s="76"/>
-      <c r="G8" s="76"/>
-      <c r="H8" s="76"/>
-      <c r="I8" s="76"/>
-      <c r="J8" s="76"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -3008,15 +3014,15 @@
         <v>6</v>
       </c>
       <c r="C9" s="6"/>
-      <c r="D9" s="77" t="s">
+      <c r="D9" s="55" t="s">
         <v>127</v>
       </c>
-      <c r="E9" s="76"/>
-      <c r="F9" s="76"/>
-      <c r="G9" s="76"/>
-      <c r="H9" s="76"/>
-      <c r="I9" s="76"/>
-      <c r="J9" s="76"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -3299,57 +3305,57 @@
       <c r="AT14" s="9"/>
     </row>
     <row r="15" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="68" t="s">
+      <c r="B15" s="69"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="59"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="59"/>
-      <c r="N15" s="59"/>
-      <c r="O15" s="59"/>
-      <c r="P15" s="59"/>
-      <c r="Q15" s="59"/>
-      <c r="R15" s="59"/>
-      <c r="S15" s="59"/>
-      <c r="T15" s="59"/>
-      <c r="U15" s="59"/>
-      <c r="V15" s="48"/>
-      <c r="W15" s="69" t="s">
+      <c r="H15" s="69"/>
+      <c r="I15" s="69"/>
+      <c r="J15" s="69"/>
+      <c r="K15" s="69"/>
+      <c r="L15" s="69"/>
+      <c r="M15" s="69"/>
+      <c r="N15" s="69"/>
+      <c r="O15" s="69"/>
+      <c r="P15" s="69"/>
+      <c r="Q15" s="69"/>
+      <c r="R15" s="69"/>
+      <c r="S15" s="69"/>
+      <c r="T15" s="69"/>
+      <c r="U15" s="69"/>
+      <c r="V15" s="60"/>
+      <c r="W15" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="X15" s="59"/>
-      <c r="Y15" s="59"/>
-      <c r="Z15" s="59"/>
-      <c r="AA15" s="59"/>
-      <c r="AB15" s="59"/>
-      <c r="AC15" s="59"/>
-      <c r="AD15" s="59"/>
-      <c r="AE15" s="48"/>
-      <c r="AF15" s="70" t="s">
+      <c r="X15" s="69"/>
+      <c r="Y15" s="69"/>
+      <c r="Z15" s="69"/>
+      <c r="AA15" s="69"/>
+      <c r="AB15" s="69"/>
+      <c r="AC15" s="69"/>
+      <c r="AD15" s="69"/>
+      <c r="AE15" s="60"/>
+      <c r="AF15" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="AG15" s="59"/>
-      <c r="AH15" s="59"/>
-      <c r="AI15" s="59"/>
-      <c r="AJ15" s="59"/>
-      <c r="AK15" s="59"/>
-      <c r="AL15" s="59"/>
-      <c r="AM15" s="48"/>
-      <c r="AN15" s="47" t="s">
+      <c r="AG15" s="69"/>
+      <c r="AH15" s="69"/>
+      <c r="AI15" s="69"/>
+      <c r="AJ15" s="69"/>
+      <c r="AK15" s="69"/>
+      <c r="AL15" s="69"/>
+      <c r="AM15" s="60"/>
+      <c r="AN15" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="AO15" s="48"/>
+      <c r="AO15" s="60"/>
       <c r="AP15" s="10"/>
       <c r="AQ15" s="10"/>
       <c r="AR15" s="10"/>
@@ -3357,47 +3363,47 @@
       <c r="AT15" s="10"/>
     </row>
     <row r="16" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="49"/>
-      <c r="B16" s="60"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="60"/>
-      <c r="J16" s="60"/>
-      <c r="K16" s="60"/>
-      <c r="L16" s="60"/>
-      <c r="M16" s="60"/>
-      <c r="N16" s="60"/>
-      <c r="O16" s="60"/>
-      <c r="P16" s="60"/>
-      <c r="Q16" s="60"/>
-      <c r="R16" s="60"/>
-      <c r="S16" s="60"/>
-      <c r="T16" s="60"/>
-      <c r="U16" s="60"/>
-      <c r="V16" s="50"/>
-      <c r="W16" s="51"/>
-      <c r="X16" s="61"/>
-      <c r="Y16" s="61"/>
-      <c r="Z16" s="61"/>
-      <c r="AA16" s="61"/>
-      <c r="AB16" s="61"/>
-      <c r="AC16" s="61"/>
-      <c r="AD16" s="61"/>
-      <c r="AE16" s="52"/>
-      <c r="AF16" s="49"/>
-      <c r="AG16" s="60"/>
-      <c r="AH16" s="60"/>
-      <c r="AI16" s="60"/>
-      <c r="AJ16" s="60"/>
-      <c r="AK16" s="60"/>
-      <c r="AL16" s="60"/>
-      <c r="AM16" s="50"/>
-      <c r="AN16" s="49"/>
-      <c r="AO16" s="50"/>
+      <c r="A16" s="61"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="70"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="70"/>
+      <c r="I16" s="70"/>
+      <c r="J16" s="70"/>
+      <c r="K16" s="70"/>
+      <c r="L16" s="70"/>
+      <c r="M16" s="70"/>
+      <c r="N16" s="70"/>
+      <c r="O16" s="70"/>
+      <c r="P16" s="70"/>
+      <c r="Q16" s="70"/>
+      <c r="R16" s="70"/>
+      <c r="S16" s="70"/>
+      <c r="T16" s="70"/>
+      <c r="U16" s="70"/>
+      <c r="V16" s="62"/>
+      <c r="W16" s="63"/>
+      <c r="X16" s="71"/>
+      <c r="Y16" s="71"/>
+      <c r="Z16" s="71"/>
+      <c r="AA16" s="71"/>
+      <c r="AB16" s="71"/>
+      <c r="AC16" s="71"/>
+      <c r="AD16" s="71"/>
+      <c r="AE16" s="64"/>
+      <c r="AF16" s="61"/>
+      <c r="AG16" s="70"/>
+      <c r="AH16" s="70"/>
+      <c r="AI16" s="70"/>
+      <c r="AJ16" s="70"/>
+      <c r="AK16" s="70"/>
+      <c r="AL16" s="70"/>
+      <c r="AM16" s="62"/>
+      <c r="AN16" s="61"/>
+      <c r="AO16" s="62"/>
       <c r="AP16" s="10"/>
       <c r="AQ16" s="10"/>
       <c r="AR16" s="10"/>
@@ -3405,53 +3411,53 @@
       <c r="AT16" s="10"/>
     </row>
     <row r="17" spans="1:46" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="51"/>
-      <c r="B17" s="61"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="61"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="61"/>
-      <c r="L17" s="61"/>
-      <c r="M17" s="61"/>
-      <c r="N17" s="61"/>
-      <c r="O17" s="61"/>
-      <c r="P17" s="61"/>
-      <c r="Q17" s="61"/>
-      <c r="R17" s="61"/>
-      <c r="S17" s="61"/>
-      <c r="T17" s="61"/>
-      <c r="U17" s="61"/>
-      <c r="V17" s="52"/>
-      <c r="W17" s="53" t="s">
+      <c r="A17" s="63"/>
+      <c r="B17" s="71"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="71"/>
+      <c r="J17" s="71"/>
+      <c r="K17" s="71"/>
+      <c r="L17" s="71"/>
+      <c r="M17" s="71"/>
+      <c r="N17" s="71"/>
+      <c r="O17" s="71"/>
+      <c r="P17" s="71"/>
+      <c r="Q17" s="71"/>
+      <c r="R17" s="71"/>
+      <c r="S17" s="71"/>
+      <c r="T17" s="71"/>
+      <c r="U17" s="71"/>
+      <c r="V17" s="64"/>
+      <c r="W17" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="X17" s="54"/>
-      <c r="Y17" s="55"/>
-      <c r="Z17" s="56" t="s">
+      <c r="X17" s="48"/>
+      <c r="Y17" s="49"/>
+      <c r="Z17" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="AA17" s="54"/>
-      <c r="AB17" s="55"/>
-      <c r="AC17" s="57" t="s">
+      <c r="AA17" s="48"/>
+      <c r="AB17" s="49"/>
+      <c r="AC17" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="AD17" s="54"/>
-      <c r="AE17" s="55"/>
-      <c r="AF17" s="51"/>
-      <c r="AG17" s="61"/>
-      <c r="AH17" s="61"/>
-      <c r="AI17" s="61"/>
-      <c r="AJ17" s="61"/>
-      <c r="AK17" s="61"/>
-      <c r="AL17" s="61"/>
-      <c r="AM17" s="52"/>
-      <c r="AN17" s="49"/>
-      <c r="AO17" s="50"/>
+      <c r="AD17" s="48"/>
+      <c r="AE17" s="49"/>
+      <c r="AF17" s="63"/>
+      <c r="AG17" s="71"/>
+      <c r="AH17" s="71"/>
+      <c r="AI17" s="71"/>
+      <c r="AJ17" s="71"/>
+      <c r="AK17" s="71"/>
+      <c r="AL17" s="71"/>
+      <c r="AM17" s="64"/>
+      <c r="AN17" s="61"/>
+      <c r="AO17" s="62"/>
       <c r="AP17" s="10"/>
       <c r="AQ17" s="10"/>
       <c r="AR17" s="10"/>
@@ -3459,69 +3465,69 @@
       <c r="AT17" s="10"/>
     </row>
     <row r="18" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A18" s="62" t="s">
+      <c r="A18" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="54"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="63" t="s">
+      <c r="B18" s="48"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="64" t="s">
+      <c r="H18" s="48"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="L18" s="54"/>
-      <c r="M18" s="54"/>
-      <c r="N18" s="55"/>
-      <c r="O18" s="65" t="s">
+      <c r="L18" s="48"/>
+      <c r="M18" s="48"/>
+      <c r="N18" s="49"/>
+      <c r="O18" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="P18" s="54"/>
-      <c r="Q18" s="55"/>
-      <c r="R18" s="71" t="s">
+      <c r="P18" s="48"/>
+      <c r="Q18" s="49"/>
+      <c r="R18" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="S18" s="54"/>
-      <c r="T18" s="54"/>
-      <c r="U18" s="54"/>
-      <c r="V18" s="55"/>
-      <c r="W18" s="72" t="s">
+      <c r="S18" s="48"/>
+      <c r="T18" s="48"/>
+      <c r="U18" s="48"/>
+      <c r="V18" s="49"/>
+      <c r="W18" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="X18" s="54"/>
-      <c r="Y18" s="55"/>
-      <c r="Z18" s="72" t="s">
+      <c r="X18" s="48"/>
+      <c r="Y18" s="49"/>
+      <c r="Z18" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="AA18" s="54"/>
-      <c r="AB18" s="55"/>
-      <c r="AC18" s="72" t="s">
+      <c r="AA18" s="48"/>
+      <c r="AB18" s="49"/>
+      <c r="AC18" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="AD18" s="54"/>
-      <c r="AE18" s="55"/>
-      <c r="AF18" s="66" t="s">
+      <c r="AD18" s="48"/>
+      <c r="AE18" s="49"/>
+      <c r="AF18" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="AG18" s="54"/>
-      <c r="AH18" s="55"/>
-      <c r="AI18" s="66" t="s">
+      <c r="AG18" s="48"/>
+      <c r="AH18" s="49"/>
+      <c r="AI18" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="AJ18" s="54"/>
-      <c r="AK18" s="55"/>
-      <c r="AL18" s="67" t="s">
+      <c r="AJ18" s="48"/>
+      <c r="AK18" s="49"/>
+      <c r="AL18" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="AM18" s="52"/>
-      <c r="AN18" s="51"/>
-      <c r="AO18" s="52"/>
+      <c r="AM18" s="64"/>
+      <c r="AN18" s="63"/>
+      <c r="AO18" s="64"/>
       <c r="AP18" s="10"/>
       <c r="AQ18" s="10"/>
       <c r="AR18" s="10"/>
@@ -3758,12 +3764,12 @@
         <v>306</v>
       </c>
       <c r="AK20" s="18" t="s">
-        <v>106</v>
+        <v>298</v>
       </c>
       <c r="AL20" s="17" t="s">
         <v>330</v>
       </c>
-      <c r="AM20" s="15" t="s">
+      <c r="AM20" s="30" t="s">
         <v>329</v>
       </c>
       <c r="AN20" s="17" t="s">
@@ -4813,8 +4819,12 @@
       <c r="AF32" s="20"/>
       <c r="AG32" s="20"/>
       <c r="AH32" s="20"/>
-      <c r="AI32" s="20"/>
-      <c r="AJ32" s="20"/>
+      <c r="AI32" s="20" t="s">
+        <v>331</v>
+      </c>
+      <c r="AJ32" s="20" t="s">
+        <v>332</v>
+      </c>
       <c r="AK32" s="20"/>
       <c r="AL32" s="20"/>
       <c r="AM32" s="20"/>
@@ -16793,16 +16803,6 @@
     <row r="1019" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="Z18:AB18"/>
-    <mergeCell ref="AC18:AE18"/>
-    <mergeCell ref="AF18:AH18"/>
-    <mergeCell ref="B4:Q4"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="D8:J8"/>
-    <mergeCell ref="D9:J9"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B6:E6"/>
     <mergeCell ref="AN15:AO18"/>
     <mergeCell ref="W17:Y17"/>
     <mergeCell ref="Z17:AB17"/>
@@ -16819,6 +16819,16 @@
     <mergeCell ref="AF15:AM17"/>
     <mergeCell ref="R18:V18"/>
     <mergeCell ref="W18:Y18"/>
+    <mergeCell ref="Z18:AB18"/>
+    <mergeCell ref="AC18:AE18"/>
+    <mergeCell ref="AF18:AH18"/>
+    <mergeCell ref="B4:Q4"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="D8:J8"/>
+    <mergeCell ref="D9:J9"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B6:E6"/>
   </mergeCells>
   <phoneticPr fontId="21" type="noConversion"/>
   <hyperlinks>
@@ -16830,6 +16840,7 @@
     <hyperlink ref="AA21" r:id="rId6" xr:uid="{1F1D9C93-0B62-4141-9155-0BF56B97D418}"/>
     <hyperlink ref="AD20" r:id="rId7" xr:uid="{11979102-4C6A-4DD8-920A-409D640D74E1}"/>
     <hyperlink ref="AG20" r:id="rId8" xr:uid="{F3612EEF-6515-43FA-9410-0BDE97984233}"/>
+    <hyperlink ref="AM20" r:id="rId9" xr:uid="{1C6FF353-7903-4FB1-B22F-D98D8E8CD6DD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -16952,17 +16963,17 @@
       <c r="V3" s="2"/>
     </row>
     <row r="4" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="84" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
@@ -17452,57 +17463,57 @@
       <c r="AT14" s="9"/>
     </row>
     <row r="15" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="68" t="s">
+      <c r="B15" s="69"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="59"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="59"/>
-      <c r="N15" s="59"/>
-      <c r="O15" s="59"/>
-      <c r="P15" s="59"/>
-      <c r="Q15" s="59"/>
-      <c r="R15" s="59"/>
-      <c r="S15" s="59"/>
-      <c r="T15" s="59"/>
-      <c r="U15" s="59"/>
-      <c r="V15" s="48"/>
-      <c r="W15" s="69" t="s">
+      <c r="H15" s="69"/>
+      <c r="I15" s="69"/>
+      <c r="J15" s="69"/>
+      <c r="K15" s="69"/>
+      <c r="L15" s="69"/>
+      <c r="M15" s="69"/>
+      <c r="N15" s="69"/>
+      <c r="O15" s="69"/>
+      <c r="P15" s="69"/>
+      <c r="Q15" s="69"/>
+      <c r="R15" s="69"/>
+      <c r="S15" s="69"/>
+      <c r="T15" s="69"/>
+      <c r="U15" s="69"/>
+      <c r="V15" s="60"/>
+      <c r="W15" s="78" t="s">
         <v>78</v>
       </c>
-      <c r="X15" s="59"/>
-      <c r="Y15" s="59"/>
-      <c r="Z15" s="59"/>
-      <c r="AA15" s="59"/>
-      <c r="AB15" s="59"/>
-      <c r="AC15" s="59"/>
-      <c r="AD15" s="59"/>
-      <c r="AE15" s="48"/>
-      <c r="AF15" s="70" t="s">
+      <c r="X15" s="69"/>
+      <c r="Y15" s="69"/>
+      <c r="Z15" s="69"/>
+      <c r="AA15" s="69"/>
+      <c r="AB15" s="69"/>
+      <c r="AC15" s="69"/>
+      <c r="AD15" s="69"/>
+      <c r="AE15" s="60"/>
+      <c r="AF15" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="AG15" s="59"/>
-      <c r="AH15" s="59"/>
-      <c r="AI15" s="59"/>
-      <c r="AJ15" s="59"/>
-      <c r="AK15" s="59"/>
-      <c r="AL15" s="59"/>
-      <c r="AM15" s="48"/>
-      <c r="AN15" s="47" t="s">
+      <c r="AG15" s="69"/>
+      <c r="AH15" s="69"/>
+      <c r="AI15" s="69"/>
+      <c r="AJ15" s="69"/>
+      <c r="AK15" s="69"/>
+      <c r="AL15" s="69"/>
+      <c r="AM15" s="60"/>
+      <c r="AN15" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="AO15" s="48"/>
+      <c r="AO15" s="60"/>
       <c r="AP15" s="10"/>
       <c r="AQ15" s="10"/>
       <c r="AR15" s="10"/>
@@ -17510,47 +17521,47 @@
       <c r="AT15" s="10"/>
     </row>
     <row r="16" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="49"/>
-      <c r="B16" s="60"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="60"/>
-      <c r="J16" s="60"/>
-      <c r="K16" s="60"/>
-      <c r="L16" s="60"/>
-      <c r="M16" s="60"/>
-      <c r="N16" s="60"/>
-      <c r="O16" s="60"/>
-      <c r="P16" s="60"/>
-      <c r="Q16" s="60"/>
-      <c r="R16" s="60"/>
-      <c r="S16" s="60"/>
-      <c r="T16" s="60"/>
-      <c r="U16" s="60"/>
-      <c r="V16" s="50"/>
-      <c r="W16" s="51"/>
-      <c r="X16" s="61"/>
-      <c r="Y16" s="61"/>
-      <c r="Z16" s="61"/>
-      <c r="AA16" s="61"/>
-      <c r="AB16" s="61"/>
-      <c r="AC16" s="61"/>
-      <c r="AD16" s="61"/>
-      <c r="AE16" s="52"/>
-      <c r="AF16" s="49"/>
-      <c r="AG16" s="60"/>
-      <c r="AH16" s="60"/>
-      <c r="AI16" s="60"/>
-      <c r="AJ16" s="60"/>
-      <c r="AK16" s="60"/>
-      <c r="AL16" s="60"/>
-      <c r="AM16" s="50"/>
-      <c r="AN16" s="49"/>
-      <c r="AO16" s="50"/>
+      <c r="A16" s="61"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="70"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="70"/>
+      <c r="I16" s="70"/>
+      <c r="J16" s="70"/>
+      <c r="K16" s="70"/>
+      <c r="L16" s="70"/>
+      <c r="M16" s="70"/>
+      <c r="N16" s="70"/>
+      <c r="O16" s="70"/>
+      <c r="P16" s="70"/>
+      <c r="Q16" s="70"/>
+      <c r="R16" s="70"/>
+      <c r="S16" s="70"/>
+      <c r="T16" s="70"/>
+      <c r="U16" s="70"/>
+      <c r="V16" s="62"/>
+      <c r="W16" s="63"/>
+      <c r="X16" s="71"/>
+      <c r="Y16" s="71"/>
+      <c r="Z16" s="71"/>
+      <c r="AA16" s="71"/>
+      <c r="AB16" s="71"/>
+      <c r="AC16" s="71"/>
+      <c r="AD16" s="71"/>
+      <c r="AE16" s="64"/>
+      <c r="AF16" s="61"/>
+      <c r="AG16" s="70"/>
+      <c r="AH16" s="70"/>
+      <c r="AI16" s="70"/>
+      <c r="AJ16" s="70"/>
+      <c r="AK16" s="70"/>
+      <c r="AL16" s="70"/>
+      <c r="AM16" s="62"/>
+      <c r="AN16" s="61"/>
+      <c r="AO16" s="62"/>
       <c r="AP16" s="10"/>
       <c r="AQ16" s="10"/>
       <c r="AR16" s="10"/>
@@ -17558,53 +17569,53 @@
       <c r="AT16" s="10"/>
     </row>
     <row r="17" spans="1:46" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="51"/>
-      <c r="B17" s="61"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="61"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="61"/>
-      <c r="L17" s="61"/>
-      <c r="M17" s="61"/>
-      <c r="N17" s="61"/>
-      <c r="O17" s="61"/>
-      <c r="P17" s="61"/>
-      <c r="Q17" s="61"/>
-      <c r="R17" s="61"/>
-      <c r="S17" s="61"/>
-      <c r="T17" s="61"/>
-      <c r="U17" s="61"/>
-      <c r="V17" s="52"/>
-      <c r="W17" s="53" t="s">
+      <c r="A17" s="63"/>
+      <c r="B17" s="71"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="71"/>
+      <c r="J17" s="71"/>
+      <c r="K17" s="71"/>
+      <c r="L17" s="71"/>
+      <c r="M17" s="71"/>
+      <c r="N17" s="71"/>
+      <c r="O17" s="71"/>
+      <c r="P17" s="71"/>
+      <c r="Q17" s="71"/>
+      <c r="R17" s="71"/>
+      <c r="S17" s="71"/>
+      <c r="T17" s="71"/>
+      <c r="U17" s="71"/>
+      <c r="V17" s="64"/>
+      <c r="W17" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="X17" s="54"/>
-      <c r="Y17" s="55"/>
-      <c r="Z17" s="56" t="s">
+      <c r="X17" s="48"/>
+      <c r="Y17" s="49"/>
+      <c r="Z17" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="AA17" s="54"/>
-      <c r="AB17" s="55"/>
-      <c r="AC17" s="57" t="s">
+      <c r="AA17" s="48"/>
+      <c r="AB17" s="49"/>
+      <c r="AC17" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="AD17" s="54"/>
-      <c r="AE17" s="55"/>
-      <c r="AF17" s="51"/>
-      <c r="AG17" s="61"/>
-      <c r="AH17" s="61"/>
-      <c r="AI17" s="61"/>
-      <c r="AJ17" s="61"/>
-      <c r="AK17" s="61"/>
-      <c r="AL17" s="61"/>
-      <c r="AM17" s="52"/>
-      <c r="AN17" s="49"/>
-      <c r="AO17" s="50"/>
+      <c r="AD17" s="48"/>
+      <c r="AE17" s="49"/>
+      <c r="AF17" s="63"/>
+      <c r="AG17" s="71"/>
+      <c r="AH17" s="71"/>
+      <c r="AI17" s="71"/>
+      <c r="AJ17" s="71"/>
+      <c r="AK17" s="71"/>
+      <c r="AL17" s="71"/>
+      <c r="AM17" s="64"/>
+      <c r="AN17" s="61"/>
+      <c r="AO17" s="62"/>
       <c r="AP17" s="10"/>
       <c r="AQ17" s="10"/>
       <c r="AR17" s="10"/>
@@ -17612,69 +17623,69 @@
       <c r="AT17" s="10"/>
     </row>
     <row r="18" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A18" s="62" t="s">
+      <c r="A18" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="54"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="63" t="s">
+      <c r="B18" s="48"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="64" t="s">
+      <c r="H18" s="48"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="L18" s="54"/>
-      <c r="M18" s="54"/>
-      <c r="N18" s="55"/>
-      <c r="O18" s="65" t="s">
+      <c r="L18" s="48"/>
+      <c r="M18" s="48"/>
+      <c r="N18" s="49"/>
+      <c r="O18" s="75" t="s">
         <v>80</v>
       </c>
-      <c r="P18" s="54"/>
-      <c r="Q18" s="55"/>
-      <c r="R18" s="71" t="s">
+      <c r="P18" s="48"/>
+      <c r="Q18" s="49"/>
+      <c r="R18" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="S18" s="54"/>
-      <c r="T18" s="54"/>
-      <c r="U18" s="54"/>
-      <c r="V18" s="55"/>
-      <c r="W18" s="72" t="s">
+      <c r="S18" s="48"/>
+      <c r="T18" s="48"/>
+      <c r="U18" s="48"/>
+      <c r="V18" s="49"/>
+      <c r="W18" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="X18" s="54"/>
-      <c r="Y18" s="55"/>
-      <c r="Z18" s="72" t="s">
+      <c r="X18" s="48"/>
+      <c r="Y18" s="49"/>
+      <c r="Z18" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="AA18" s="54"/>
-      <c r="AB18" s="55"/>
-      <c r="AC18" s="72" t="s">
+      <c r="AA18" s="48"/>
+      <c r="AB18" s="49"/>
+      <c r="AC18" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="AD18" s="54"/>
-      <c r="AE18" s="55"/>
-      <c r="AF18" s="66" t="s">
+      <c r="AD18" s="48"/>
+      <c r="AE18" s="49"/>
+      <c r="AF18" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="AG18" s="54"/>
-      <c r="AH18" s="55"/>
-      <c r="AI18" s="66" t="s">
+      <c r="AG18" s="48"/>
+      <c r="AH18" s="49"/>
+      <c r="AI18" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="AJ18" s="54"/>
-      <c r="AK18" s="55"/>
-      <c r="AL18" s="67" t="s">
+      <c r="AJ18" s="48"/>
+      <c r="AK18" s="49"/>
+      <c r="AL18" s="76" t="s">
         <v>85</v>
       </c>
-      <c r="AM18" s="52"/>
-      <c r="AN18" s="51"/>
-      <c r="AO18" s="52"/>
+      <c r="AM18" s="64"/>
+      <c r="AN18" s="63"/>
+      <c r="AO18" s="64"/>
       <c r="AP18" s="10"/>
       <c r="AQ18" s="10"/>
       <c r="AR18" s="10"/>
@@ -17900,55 +17911,55 @@
       <c r="AT20" s="19"/>
     </row>
     <row r="21" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="82" t="s">
+      <c r="A21" s="81" t="s">
         <v>93</v>
       </c>
-      <c r="B21" s="82" t="s">
+      <c r="B21" s="81" t="s">
         <v>94</v>
       </c>
-      <c r="C21" s="82" t="s">
+      <c r="C21" s="81" t="s">
         <v>95</v>
       </c>
-      <c r="D21" s="82" t="s">
+      <c r="D21" s="81" t="s">
         <v>96</v>
       </c>
-      <c r="E21" s="85">
+      <c r="E21" s="86">
         <v>44650</v>
       </c>
-      <c r="F21" s="82">
+      <c r="F21" s="81">
         <v>1</v>
       </c>
-      <c r="G21" s="82" t="s">
+      <c r="G21" s="81" t="s">
         <v>97</v>
       </c>
-      <c r="H21" s="82" t="s">
+      <c r="H21" s="81" t="s">
         <v>98</v>
       </c>
-      <c r="I21" s="82" t="s">
+      <c r="I21" s="81" t="s">
         <v>99</v>
       </c>
-      <c r="J21" s="82">
+      <c r="J21" s="81">
         <v>1</v>
       </c>
-      <c r="K21" s="86" t="s">
+      <c r="K21" s="83" t="s">
         <v>100</v>
       </c>
-      <c r="L21" s="82" t="s">
+      <c r="L21" s="81" t="s">
         <v>101</v>
       </c>
-      <c r="M21" s="82" t="s">
+      <c r="M21" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="N21" s="82" t="s">
+      <c r="N21" s="81" t="s">
         <v>103</v>
       </c>
-      <c r="O21" s="82" t="s">
+      <c r="O21" s="81" t="s">
         <v>104</v>
       </c>
-      <c r="P21" s="82" t="s">
+      <c r="P21" s="81" t="s">
         <v>105</v>
       </c>
-      <c r="Q21" s="82" t="s">
+      <c r="Q21" s="81" t="s">
         <v>106</v>
       </c>
       <c r="R21" s="20" t="s">
@@ -17994,23 +18005,23 @@
       <c r="AT21" s="2"/>
     </row>
     <row r="22" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="84"/>
-      <c r="B22" s="84"/>
-      <c r="C22" s="84"/>
-      <c r="D22" s="84"/>
-      <c r="E22" s="84"/>
-      <c r="F22" s="84"/>
-      <c r="G22" s="83"/>
-      <c r="H22" s="83"/>
-      <c r="I22" s="83"/>
-      <c r="J22" s="83"/>
-      <c r="K22" s="52"/>
-      <c r="L22" s="83"/>
-      <c r="M22" s="83"/>
-      <c r="N22" s="83"/>
-      <c r="O22" s="83"/>
-      <c r="P22" s="83"/>
-      <c r="Q22" s="83"/>
+      <c r="A22" s="85"/>
+      <c r="B22" s="85"/>
+      <c r="C22" s="85"/>
+      <c r="D22" s="85"/>
+      <c r="E22" s="85"/>
+      <c r="F22" s="85"/>
+      <c r="G22" s="82"/>
+      <c r="H22" s="82"/>
+      <c r="I22" s="82"/>
+      <c r="J22" s="82"/>
+      <c r="K22" s="64"/>
+      <c r="L22" s="82"/>
+      <c r="M22" s="82"/>
+      <c r="N22" s="82"/>
+      <c r="O22" s="82"/>
+      <c r="P22" s="82"/>
+      <c r="Q22" s="82"/>
       <c r="R22" s="20" t="s">
         <v>113</v>
       </c>
@@ -18044,12 +18055,12 @@
       <c r="AT22" s="2"/>
     </row>
     <row r="23" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="84"/>
-      <c r="B23" s="84"/>
-      <c r="C23" s="84"/>
-      <c r="D23" s="84"/>
-      <c r="E23" s="84"/>
-      <c r="F23" s="84"/>
+      <c r="A23" s="85"/>
+      <c r="B23" s="85"/>
+      <c r="C23" s="85"/>
+      <c r="D23" s="85"/>
+      <c r="E23" s="85"/>
+      <c r="F23" s="85"/>
       <c r="G23" s="20" t="s">
         <v>114</v>
       </c>
@@ -18100,12 +18111,12 @@
       <c r="AT23" s="2"/>
     </row>
     <row r="24" spans="1:46" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="83"/>
-      <c r="B24" s="83"/>
-      <c r="C24" s="83"/>
-      <c r="D24" s="83"/>
-      <c r="E24" s="83"/>
-      <c r="F24" s="83"/>
+      <c r="A24" s="82"/>
+      <c r="B24" s="82"/>
+      <c r="C24" s="82"/>
+      <c r="D24" s="82"/>
+      <c r="E24" s="82"/>
+      <c r="F24" s="82"/>
       <c r="G24" s="20" t="s">
         <v>117</v>
       </c>
@@ -29353,15 +29364,22 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="P21:P22"/>
-    <mergeCell ref="Q21:Q22"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="L21:L22"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="N21:N22"/>
-    <mergeCell ref="O21:O22"/>
+    <mergeCell ref="AF15:AM17"/>
+    <mergeCell ref="AN15:AO18"/>
+    <mergeCell ref="W17:Y17"/>
+    <mergeCell ref="Z17:AB17"/>
+    <mergeCell ref="AC17:AE17"/>
+    <mergeCell ref="W18:Y18"/>
+    <mergeCell ref="Z18:AB18"/>
+    <mergeCell ref="AC18:AE18"/>
+    <mergeCell ref="AF18:AH18"/>
+    <mergeCell ref="AI18:AK18"/>
+    <mergeCell ref="AL18:AM18"/>
+    <mergeCell ref="K18:N18"/>
+    <mergeCell ref="O18:Q18"/>
+    <mergeCell ref="R18:V18"/>
+    <mergeCell ref="G15:V17"/>
+    <mergeCell ref="W15:AE16"/>
     <mergeCell ref="A4:I4"/>
     <mergeCell ref="G21:G22"/>
     <mergeCell ref="H21:H22"/>
@@ -29374,22 +29392,15 @@
     <mergeCell ref="A21:A24"/>
     <mergeCell ref="A15:F17"/>
     <mergeCell ref="A18:F18"/>
-    <mergeCell ref="K18:N18"/>
-    <mergeCell ref="O18:Q18"/>
-    <mergeCell ref="R18:V18"/>
-    <mergeCell ref="G15:V17"/>
-    <mergeCell ref="W15:AE16"/>
-    <mergeCell ref="AF15:AM17"/>
-    <mergeCell ref="AN15:AO18"/>
-    <mergeCell ref="W17:Y17"/>
-    <mergeCell ref="Z17:AB17"/>
-    <mergeCell ref="AC17:AE17"/>
-    <mergeCell ref="W18:Y18"/>
-    <mergeCell ref="Z18:AB18"/>
-    <mergeCell ref="AC18:AE18"/>
-    <mergeCell ref="AF18:AH18"/>
-    <mergeCell ref="AI18:AK18"/>
-    <mergeCell ref="AL18:AM18"/>
+    <mergeCell ref="P21:P22"/>
+    <mergeCell ref="Q21:Q22"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="N21:N22"/>
+    <mergeCell ref="O21:O22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
working login log out button
</commit_message>
<xml_diff>
--- a/misc/CMSC 128 Requirements Traceability Matrix for SHUFFLE (Eulin).xlsx
+++ b/misc/CMSC 128 Requirements Traceability Matrix for SHUFFLE (Eulin).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\shuffle\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447C3571-5F1D-4056-974F-20239E0BEF73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074E5276-3E4D-472E-91A8-B44408CEE925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RTM" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="352">
   <si>
     <t>Requirements Traceability Matrix (Sample Template)</t>
   </si>
@@ -1272,15 +1272,9 @@
     <t>ts101</t>
   </si>
   <si>
-    <t>As a user, I want to be able to peak through the topmost cards (to up to 7 cards)</t>
-  </si>
-  <si>
     <t>ts102</t>
   </si>
   <si>
-    <t>As a user, I want to be able to reduce the number of peaked cards</t>
-  </si>
-  <si>
     <t>As a user, I want to be able to shift (bring to bottom) the topmost card</t>
   </si>
   <si>
@@ -1876,6 +1870,21 @@
   </si>
   <si>
     <t>https://docs.google.com/spreadsheets/d/1PeDh14bQqVsLShnfbeQ1JbiSmwicG1gsVKFPQP0nRq4/edit?usp=sharing</t>
+  </si>
+  <si>
+    <t>As a user, I want to be able to peek through the topmost cards (to up to 7 cards)</t>
+  </si>
+  <si>
+    <t>As a user, I want to be able to reduce the number of peeked cards</t>
+  </si>
+  <si>
+    <t>As a user, I should be able to create an account</t>
+  </si>
+  <si>
+    <t>ts302</t>
+  </si>
+  <si>
+    <t>As a user, I should be able to log in to my account</t>
   </si>
 </sst>
 </file>
@@ -2422,62 +2431,12 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2504,12 +2463,62 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2728,8 +2737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AT1019"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N15" zoomScale="108" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="V27" sqref="V27"/>
+    <sheetView tabSelected="1" topLeftCell="F19" zoomScale="108" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2820,10 +2829,10 @@
       <c r="A3" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="C3" s="74"/>
+      <c r="C3" s="52"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -2848,24 +2857,24 @@
       <c r="A4" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="51" t="s">
         <v>129</v>
       </c>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="73"/>
-      <c r="N4" s="73"/>
-      <c r="O4" s="73"/>
-      <c r="P4" s="73"/>
-      <c r="Q4" s="73"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="51"/>
+      <c r="N4" s="51"/>
+      <c r="O4" s="51"/>
+      <c r="P4" s="51"/>
+      <c r="Q4" s="51"/>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
@@ -2876,11 +2885,11 @@
       <c r="A5" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B5" s="75" t="s">
+      <c r="B5" s="53" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -2904,12 +2913,12 @@
       <c r="A6" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B6" s="80" t="s">
+      <c r="B6" s="58" t="s">
         <v>125</v>
       </c>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
@@ -2956,13 +2965,13 @@
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="78" t="s">
+      <c r="B7" s="56" t="s">
         <v>126</v>
       </c>
-      <c r="C7" s="79"/>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="79"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -3010,15 +3019,15 @@
         <v>4</v>
       </c>
       <c r="C8" s="6"/>
-      <c r="D8" s="76" t="s">
+      <c r="D8" s="54" t="s">
         <v>128</v>
       </c>
-      <c r="E8" s="76"/>
-      <c r="F8" s="76"/>
-      <c r="G8" s="76"/>
-      <c r="H8" s="76"/>
-      <c r="I8" s="76"/>
-      <c r="J8" s="76"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -3062,15 +3071,15 @@
         <v>6</v>
       </c>
       <c r="C9" s="6"/>
-      <c r="D9" s="77" t="s">
+      <c r="D9" s="55" t="s">
         <v>127</v>
       </c>
-      <c r="E9" s="76"/>
-      <c r="F9" s="76"/>
-      <c r="G9" s="76"/>
-      <c r="H9" s="76"/>
-      <c r="I9" s="76"/>
-      <c r="J9" s="76"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="54"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -3353,57 +3362,57 @@
       <c r="AT14" s="9"/>
     </row>
     <row r="15" spans="1:46" ht="12.75" customHeight="1">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="68" t="s">
+      <c r="B15" s="69"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="59"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="59"/>
-      <c r="N15" s="59"/>
-      <c r="O15" s="59"/>
-      <c r="P15" s="59"/>
-      <c r="Q15" s="59"/>
-      <c r="R15" s="59"/>
-      <c r="S15" s="59"/>
-      <c r="T15" s="59"/>
-      <c r="U15" s="59"/>
-      <c r="V15" s="48"/>
-      <c r="W15" s="69" t="s">
+      <c r="H15" s="69"/>
+      <c r="I15" s="69"/>
+      <c r="J15" s="69"/>
+      <c r="K15" s="69"/>
+      <c r="L15" s="69"/>
+      <c r="M15" s="69"/>
+      <c r="N15" s="69"/>
+      <c r="O15" s="69"/>
+      <c r="P15" s="69"/>
+      <c r="Q15" s="69"/>
+      <c r="R15" s="69"/>
+      <c r="S15" s="69"/>
+      <c r="T15" s="69"/>
+      <c r="U15" s="69"/>
+      <c r="V15" s="60"/>
+      <c r="W15" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="X15" s="59"/>
-      <c r="Y15" s="59"/>
-      <c r="Z15" s="59"/>
-      <c r="AA15" s="59"/>
-      <c r="AB15" s="59"/>
-      <c r="AC15" s="59"/>
-      <c r="AD15" s="59"/>
-      <c r="AE15" s="48"/>
-      <c r="AF15" s="70" t="s">
+      <c r="X15" s="69"/>
+      <c r="Y15" s="69"/>
+      <c r="Z15" s="69"/>
+      <c r="AA15" s="69"/>
+      <c r="AB15" s="69"/>
+      <c r="AC15" s="69"/>
+      <c r="AD15" s="69"/>
+      <c r="AE15" s="60"/>
+      <c r="AF15" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="AG15" s="59"/>
-      <c r="AH15" s="59"/>
-      <c r="AI15" s="59"/>
-      <c r="AJ15" s="59"/>
-      <c r="AK15" s="59"/>
-      <c r="AL15" s="59"/>
-      <c r="AM15" s="48"/>
-      <c r="AN15" s="47" t="s">
+      <c r="AG15" s="69"/>
+      <c r="AH15" s="69"/>
+      <c r="AI15" s="69"/>
+      <c r="AJ15" s="69"/>
+      <c r="AK15" s="69"/>
+      <c r="AL15" s="69"/>
+      <c r="AM15" s="60"/>
+      <c r="AN15" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="AO15" s="48"/>
+      <c r="AO15" s="60"/>
       <c r="AP15" s="10"/>
       <c r="AQ15" s="10"/>
       <c r="AR15" s="10"/>
@@ -3411,47 +3420,47 @@
       <c r="AT15" s="10"/>
     </row>
     <row r="16" spans="1:46" ht="12.75" customHeight="1">
-      <c r="A16" s="49"/>
-      <c r="B16" s="60"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="60"/>
-      <c r="J16" s="60"/>
-      <c r="K16" s="60"/>
-      <c r="L16" s="60"/>
-      <c r="M16" s="60"/>
-      <c r="N16" s="60"/>
-      <c r="O16" s="60"/>
-      <c r="P16" s="60"/>
-      <c r="Q16" s="60"/>
-      <c r="R16" s="60"/>
-      <c r="S16" s="60"/>
-      <c r="T16" s="60"/>
-      <c r="U16" s="60"/>
-      <c r="V16" s="50"/>
-      <c r="W16" s="51"/>
-      <c r="X16" s="61"/>
-      <c r="Y16" s="61"/>
-      <c r="Z16" s="61"/>
-      <c r="AA16" s="61"/>
-      <c r="AB16" s="61"/>
-      <c r="AC16" s="61"/>
-      <c r="AD16" s="61"/>
-      <c r="AE16" s="52"/>
-      <c r="AF16" s="49"/>
-      <c r="AG16" s="60"/>
-      <c r="AH16" s="60"/>
-      <c r="AI16" s="60"/>
-      <c r="AJ16" s="60"/>
-      <c r="AK16" s="60"/>
-      <c r="AL16" s="60"/>
-      <c r="AM16" s="50"/>
-      <c r="AN16" s="49"/>
-      <c r="AO16" s="50"/>
+      <c r="A16" s="61"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="70"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="70"/>
+      <c r="I16" s="70"/>
+      <c r="J16" s="70"/>
+      <c r="K16" s="70"/>
+      <c r="L16" s="70"/>
+      <c r="M16" s="70"/>
+      <c r="N16" s="70"/>
+      <c r="O16" s="70"/>
+      <c r="P16" s="70"/>
+      <c r="Q16" s="70"/>
+      <c r="R16" s="70"/>
+      <c r="S16" s="70"/>
+      <c r="T16" s="70"/>
+      <c r="U16" s="70"/>
+      <c r="V16" s="62"/>
+      <c r="W16" s="63"/>
+      <c r="X16" s="71"/>
+      <c r="Y16" s="71"/>
+      <c r="Z16" s="71"/>
+      <c r="AA16" s="71"/>
+      <c r="AB16" s="71"/>
+      <c r="AC16" s="71"/>
+      <c r="AD16" s="71"/>
+      <c r="AE16" s="64"/>
+      <c r="AF16" s="61"/>
+      <c r="AG16" s="70"/>
+      <c r="AH16" s="70"/>
+      <c r="AI16" s="70"/>
+      <c r="AJ16" s="70"/>
+      <c r="AK16" s="70"/>
+      <c r="AL16" s="70"/>
+      <c r="AM16" s="62"/>
+      <c r="AN16" s="61"/>
+      <c r="AO16" s="62"/>
       <c r="AP16" s="10"/>
       <c r="AQ16" s="10"/>
       <c r="AR16" s="10"/>
@@ -3459,53 +3468,53 @@
       <c r="AT16" s="10"/>
     </row>
     <row r="17" spans="1:46" ht="26.25" customHeight="1">
-      <c r="A17" s="51"/>
-      <c r="B17" s="61"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="61"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="61"/>
-      <c r="L17" s="61"/>
-      <c r="M17" s="61"/>
-      <c r="N17" s="61"/>
-      <c r="O17" s="61"/>
-      <c r="P17" s="61"/>
-      <c r="Q17" s="61"/>
-      <c r="R17" s="61"/>
-      <c r="S17" s="61"/>
-      <c r="T17" s="61"/>
-      <c r="U17" s="61"/>
-      <c r="V17" s="52"/>
-      <c r="W17" s="53" t="s">
+      <c r="A17" s="63"/>
+      <c r="B17" s="71"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="71"/>
+      <c r="J17" s="71"/>
+      <c r="K17" s="71"/>
+      <c r="L17" s="71"/>
+      <c r="M17" s="71"/>
+      <c r="N17" s="71"/>
+      <c r="O17" s="71"/>
+      <c r="P17" s="71"/>
+      <c r="Q17" s="71"/>
+      <c r="R17" s="71"/>
+      <c r="S17" s="71"/>
+      <c r="T17" s="71"/>
+      <c r="U17" s="71"/>
+      <c r="V17" s="64"/>
+      <c r="W17" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="X17" s="54"/>
-      <c r="Y17" s="55"/>
-      <c r="Z17" s="56" t="s">
+      <c r="X17" s="48"/>
+      <c r="Y17" s="49"/>
+      <c r="Z17" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="AA17" s="54"/>
-      <c r="AB17" s="55"/>
-      <c r="AC17" s="57" t="s">
+      <c r="AA17" s="48"/>
+      <c r="AB17" s="49"/>
+      <c r="AC17" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="AD17" s="54"/>
-      <c r="AE17" s="55"/>
-      <c r="AF17" s="51"/>
-      <c r="AG17" s="61"/>
-      <c r="AH17" s="61"/>
-      <c r="AI17" s="61"/>
-      <c r="AJ17" s="61"/>
-      <c r="AK17" s="61"/>
-      <c r="AL17" s="61"/>
-      <c r="AM17" s="52"/>
-      <c r="AN17" s="49"/>
-      <c r="AO17" s="50"/>
+      <c r="AD17" s="48"/>
+      <c r="AE17" s="49"/>
+      <c r="AF17" s="63"/>
+      <c r="AG17" s="71"/>
+      <c r="AH17" s="71"/>
+      <c r="AI17" s="71"/>
+      <c r="AJ17" s="71"/>
+      <c r="AK17" s="71"/>
+      <c r="AL17" s="71"/>
+      <c r="AM17" s="64"/>
+      <c r="AN17" s="61"/>
+      <c r="AO17" s="62"/>
       <c r="AP17" s="10"/>
       <c r="AQ17" s="10"/>
       <c r="AR17" s="10"/>
@@ -3513,69 +3522,69 @@
       <c r="AT17" s="10"/>
     </row>
     <row r="18" spans="1:46">
-      <c r="A18" s="62" t="s">
+      <c r="A18" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="54"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="63" t="s">
+      <c r="B18" s="48"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="64" t="s">
+      <c r="H18" s="48"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="L18" s="54"/>
-      <c r="M18" s="54"/>
-      <c r="N18" s="55"/>
-      <c r="O18" s="65" t="s">
+      <c r="L18" s="48"/>
+      <c r="M18" s="48"/>
+      <c r="N18" s="49"/>
+      <c r="O18" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="P18" s="54"/>
-      <c r="Q18" s="55"/>
-      <c r="R18" s="71" t="s">
+      <c r="P18" s="48"/>
+      <c r="Q18" s="49"/>
+      <c r="R18" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="S18" s="54"/>
-      <c r="T18" s="54"/>
-      <c r="U18" s="54"/>
-      <c r="V18" s="55"/>
-      <c r="W18" s="72" t="s">
+      <c r="S18" s="48"/>
+      <c r="T18" s="48"/>
+      <c r="U18" s="48"/>
+      <c r="V18" s="49"/>
+      <c r="W18" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="X18" s="54"/>
-      <c r="Y18" s="55"/>
-      <c r="Z18" s="72" t="s">
+      <c r="X18" s="48"/>
+      <c r="Y18" s="49"/>
+      <c r="Z18" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="AA18" s="54"/>
-      <c r="AB18" s="55"/>
-      <c r="AC18" s="72" t="s">
+      <c r="AA18" s="48"/>
+      <c r="AB18" s="49"/>
+      <c r="AC18" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="AD18" s="54"/>
-      <c r="AE18" s="55"/>
-      <c r="AF18" s="66" t="s">
+      <c r="AD18" s="48"/>
+      <c r="AE18" s="49"/>
+      <c r="AF18" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="AG18" s="54"/>
-      <c r="AH18" s="55"/>
-      <c r="AI18" s="66" t="s">
+      <c r="AG18" s="48"/>
+      <c r="AH18" s="49"/>
+      <c r="AI18" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="AJ18" s="54"/>
-      <c r="AK18" s="55"/>
-      <c r="AL18" s="67" t="s">
+      <c r="AJ18" s="48"/>
+      <c r="AK18" s="49"/>
+      <c r="AL18" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="AM18" s="52"/>
-      <c r="AN18" s="51"/>
-      <c r="AO18" s="52"/>
+      <c r="AM18" s="64"/>
+      <c r="AN18" s="63"/>
+      <c r="AO18" s="64"/>
       <c r="AP18" s="10"/>
       <c r="AQ18" s="10"/>
       <c r="AR18" s="10"/>
@@ -3732,101 +3741,101 @@
         <v>58</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H20" s="29" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I20" s="16">
         <v>2</v>
       </c>
       <c r="J20" s="36" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K20" s="39" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="L20" s="39" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="M20" s="39" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="N20" s="39" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="O20" s="37" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="P20" s="15" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="Q20" s="16" t="s">
         <v>106</v>
       </c>
       <c r="R20" s="17" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="S20" s="30" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="T20" s="15" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="U20" s="15" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="V20" s="15"/>
       <c r="W20" s="15" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="X20" s="30" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="Y20" s="16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="Z20" s="17" t="s">
         <v>53</v>
       </c>
       <c r="AA20" s="30" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AB20" s="16" t="s">
+        <v>296</v>
+      </c>
+      <c r="AC20" s="15" t="s">
+        <v>300</v>
+      </c>
+      <c r="AD20" s="30" t="s">
+        <v>299</v>
+      </c>
+      <c r="AE20" s="16" t="s">
         <v>298</v>
       </c>
-      <c r="AC20" s="15" t="s">
+      <c r="AF20" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="AG20" s="30" t="s">
         <v>302</v>
       </c>
-      <c r="AD20" s="30" t="s">
-        <v>301</v>
-      </c>
-      <c r="AE20" s="16" t="s">
-        <v>300</v>
-      </c>
-      <c r="AF20" s="17" t="s">
+      <c r="AH20" s="16" t="s">
+        <v>296</v>
+      </c>
+      <c r="AI20" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="AG20" s="30" t="s">
+      <c r="AJ20" s="17" t="s">
         <v>304</v>
       </c>
-      <c r="AH20" s="16" t="s">
-        <v>298</v>
-      </c>
-      <c r="AI20" s="17" t="s">
-        <v>305</v>
-      </c>
-      <c r="AJ20" s="17" t="s">
-        <v>306</v>
-      </c>
       <c r="AK20" s="18" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AL20" s="17" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="AM20" s="30" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="AN20" s="17" t="s">
         <v>53</v>
@@ -3858,49 +3867,49 @@
         <v>1</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H21" s="20" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I21" s="20">
         <v>2</v>
       </c>
       <c r="J21" s="36" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K21" s="39" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="L21" s="39" t="s">
+        <v>216</v>
+      </c>
+      <c r="M21" s="39" t="s">
         <v>218</v>
       </c>
-      <c r="M21" s="39" t="s">
-        <v>220</v>
-      </c>
       <c r="N21" s="39" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="O21" s="26" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="P21" s="20" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="Q21" s="20" t="s">
         <v>106</v>
       </c>
       <c r="R21" s="20" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="S21" s="30" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="T21" s="20" t="s">
         <v>108</v>
       </c>
       <c r="U21" s="15" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="V21" s="20"/>
       <c r="W21" s="20"/>
@@ -3908,10 +3917,10 @@
       <c r="Y21" s="20"/>
       <c r="Z21" s="20"/>
       <c r="AA21" s="30" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AB21" s="16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AC21" s="20"/>
       <c r="AD21" s="20"/>
@@ -3920,10 +3929,10 @@
       <c r="AG21" s="20"/>
       <c r="AH21" s="20"/>
       <c r="AI21" s="20" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="AJ21" s="20" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="AK21" s="18" t="s">
         <v>106</v>
@@ -3958,49 +3967,49 @@
         <v>1</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H22" s="20" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I22" s="20">
         <v>2</v>
       </c>
       <c r="J22" s="36" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K22" s="39" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="L22" s="39" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="M22" s="39" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="N22" s="39" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="O22" s="26" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="P22" s="20" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="Q22" s="20" t="s">
         <v>106</v>
       </c>
       <c r="R22" s="20" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="S22" s="30" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="T22" s="20" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="U22" s="15" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="V22" s="20"/>
       <c r="W22" s="20"/>
@@ -4008,10 +4017,10 @@
       <c r="Y22" s="20"/>
       <c r="Z22" s="20"/>
       <c r="AA22" s="20" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AB22" s="16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AC22" s="20"/>
       <c r="AD22" s="20"/>
@@ -4020,10 +4029,10 @@
       <c r="AG22" s="20"/>
       <c r="AH22" s="20"/>
       <c r="AI22" s="20" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="AJ22" s="20" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="AK22" s="18" t="s">
         <v>106</v>
@@ -4058,49 +4067,49 @@
         <v>1</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H23" s="20" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I23" s="20">
         <v>2</v>
       </c>
       <c r="J23" s="36" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K23" s="39" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="L23" s="39" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="M23" s="39" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="N23" s="39" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="O23" s="26" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="P23" s="20" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="Q23" s="20" t="s">
         <v>106</v>
       </c>
       <c r="R23" s="20" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="S23" s="30" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="T23" s="20" t="s">
         <v>108</v>
       </c>
       <c r="U23" s="15" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="V23" s="20"/>
       <c r="W23" s="20"/>
@@ -4108,10 +4117,10 @@
       <c r="Y23" s="20"/>
       <c r="Z23" s="20"/>
       <c r="AA23" s="20" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AB23" s="16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AC23" s="20"/>
       <c r="AD23" s="20"/>
@@ -4120,10 +4129,10 @@
       <c r="AG23" s="20"/>
       <c r="AH23" s="20"/>
       <c r="AI23" s="20" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="AJ23" s="20" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="AK23" s="18" t="s">
         <v>106</v>
@@ -4158,49 +4167,49 @@
         <v>1</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H24" s="20" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I24" s="20">
         <v>2</v>
       </c>
       <c r="J24" s="36" t="s">
+        <v>204</v>
+      </c>
+      <c r="K24" s="40" t="s">
+        <v>263</v>
+      </c>
+      <c r="L24" s="40" t="s">
+        <v>205</v>
+      </c>
+      <c r="M24" s="41" t="s">
         <v>206</v>
       </c>
-      <c r="K24" s="40" t="s">
-        <v>265</v>
-      </c>
-      <c r="L24" s="40" t="s">
-        <v>207</v>
-      </c>
-      <c r="M24" s="41" t="s">
-        <v>208</v>
-      </c>
       <c r="N24" s="41" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="O24" s="26" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="P24" s="20" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="Q24" s="20" t="s">
         <v>106</v>
       </c>
       <c r="R24" s="20" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="S24" s="30" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="T24" s="20" t="s">
         <v>108</v>
       </c>
       <c r="U24" s="15" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="V24" s="20"/>
       <c r="W24" s="20"/>
@@ -4208,10 +4217,10 @@
       <c r="Y24" s="20"/>
       <c r="Z24" s="20"/>
       <c r="AA24" s="20" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AB24" s="16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AC24" s="20"/>
       <c r="AD24" s="20"/>
@@ -4220,10 +4229,10 @@
       <c r="AG24" s="20"/>
       <c r="AH24" s="20"/>
       <c r="AI24" s="20" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="AJ24" s="20" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="AK24" s="18" t="s">
         <v>106</v>
@@ -4258,43 +4267,43 @@
         <v>1</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H25" s="20" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I25" s="20">
         <v>2</v>
       </c>
       <c r="J25" s="15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K25" s="42" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L25" s="42" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="M25" s="43" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="N25" s="42" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="O25" s="20"/>
       <c r="P25" s="20"/>
       <c r="Q25" s="20"/>
       <c r="R25" s="20" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="S25" s="30" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="T25" s="20" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="U25" s="15" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="V25" s="20"/>
       <c r="W25" s="20"/>
@@ -4302,10 +4311,10 @@
       <c r="Y25" s="20"/>
       <c r="Z25" s="20"/>
       <c r="AA25" s="20" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AB25" s="16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AC25" s="20"/>
       <c r="AD25" s="20"/>
@@ -4314,10 +4323,10 @@
       <c r="AG25" s="20"/>
       <c r="AH25" s="20"/>
       <c r="AI25" s="20" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="AJ25" s="20" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="AK25" s="18" t="s">
         <v>106</v>
@@ -4355,40 +4364,40 @@
         <v>146</v>
       </c>
       <c r="H26" s="30" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I26" s="20">
         <v>2</v>
       </c>
       <c r="J26" s="15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K26" s="39" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="L26" s="39" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M26" s="44" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="N26" s="39" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="O26" s="20"/>
       <c r="P26" s="20"/>
       <c r="Q26" s="20"/>
       <c r="R26" s="20" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="S26" s="30" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="T26" s="20" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="U26" s="15" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="V26" s="20"/>
       <c r="W26" s="20"/>
@@ -4396,10 +4405,10 @@
       <c r="Y26" s="20"/>
       <c r="Z26" s="20"/>
       <c r="AA26" s="20" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AB26" s="16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AC26" s="20"/>
       <c r="AD26" s="20"/>
@@ -4408,10 +4417,10 @@
       <c r="AG26" s="20"/>
       <c r="AH26" s="20"/>
       <c r="AI26" s="20" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AJ26" s="20" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="AK26" s="18" t="s">
         <v>106</v>
@@ -4446,43 +4455,43 @@
         <v>1</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H27" s="20" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I27" s="20">
         <v>2</v>
       </c>
       <c r="J27" s="15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K27" s="40" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="L27" s="40" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="M27" s="41" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="N27" s="40" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="O27" s="20"/>
       <c r="P27" s="20"/>
       <c r="Q27" s="20"/>
       <c r="R27" s="20" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="S27" s="30" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="T27" s="20" t="s">
         <v>108</v>
       </c>
       <c r="U27" s="15" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="V27" s="20"/>
       <c r="W27" s="20"/>
@@ -4490,10 +4499,10 @@
       <c r="Y27" s="20"/>
       <c r="Z27" s="20"/>
       <c r="AA27" s="20" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AB27" s="16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AC27" s="20"/>
       <c r="AD27" s="20"/>
@@ -4502,10 +4511,10 @@
       <c r="AG27" s="20"/>
       <c r="AH27" s="20"/>
       <c r="AI27" s="20" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="AJ27" s="20" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="AK27" s="18" t="s">
         <v>106</v>
@@ -4525,7 +4534,7 @@
         <v>146</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>147</v>
+        <v>347</v>
       </c>
       <c r="C28" s="20" t="s">
         <v>115</v>
@@ -4540,43 +4549,43 @@
         <v>1</v>
       </c>
       <c r="G28" s="15" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H28" s="20" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I28" s="20">
         <v>2</v>
       </c>
       <c r="J28" s="15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K28" s="42" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="L28" s="42" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="M28" s="43" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="N28" s="42" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="O28" s="20"/>
       <c r="P28" s="20"/>
       <c r="Q28" s="20"/>
       <c r="R28" s="20" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="S28" s="30" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="T28" s="20" t="s">
         <v>108</v>
       </c>
       <c r="U28" s="15" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="V28" s="20"/>
       <c r="W28" s="20"/>
@@ -4584,10 +4593,10 @@
       <c r="Y28" s="20"/>
       <c r="Z28" s="20"/>
       <c r="AA28" s="20" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AB28" s="16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AC28" s="20"/>
       <c r="AD28" s="20"/>
@@ -4596,10 +4605,10 @@
       <c r="AG28" s="20"/>
       <c r="AH28" s="20"/>
       <c r="AI28" s="20" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="AJ28" s="20" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="AK28" s="18" t="s">
         <v>106</v>
@@ -4616,10 +4625,10 @@
     </row>
     <row r="29" spans="1:46" ht="19.5" customHeight="1">
       <c r="A29" s="20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>149</v>
+        <v>348</v>
       </c>
       <c r="C29" s="20" t="s">
         <v>115</v>
@@ -4634,43 +4643,43 @@
         <v>1</v>
       </c>
       <c r="G29" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H29" s="20" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="I29" s="20">
         <v>2</v>
       </c>
       <c r="J29" s="36" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K29" s="39" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="L29" s="39" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="M29" s="39" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="N29" s="39" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="O29" s="26"/>
       <c r="P29" s="20"/>
       <c r="Q29" s="20"/>
       <c r="R29" s="20" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="S29" s="30" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="T29" s="20" t="s">
         <v>108</v>
       </c>
       <c r="U29" s="15" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="V29" s="20"/>
       <c r="W29" s="20"/>
@@ -4678,10 +4687,10 @@
       <c r="Y29" s="20"/>
       <c r="Z29" s="20"/>
       <c r="AA29" s="20" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AB29" s="16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AC29" s="20"/>
       <c r="AD29" s="20"/>
@@ -4690,10 +4699,10 @@
       <c r="AG29" s="20"/>
       <c r="AH29" s="20"/>
       <c r="AI29" s="20" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="AJ29" s="20" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="AK29" s="18" t="s">
         <v>106</v>
@@ -4710,10 +4719,10 @@
     </row>
     <row r="30" spans="1:46" ht="19.5" customHeight="1">
       <c r="A30" s="20" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C30" s="20" t="s">
         <v>115</v>
@@ -4728,43 +4737,43 @@
         <v>1</v>
       </c>
       <c r="G30" s="15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H30" s="20" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I30" s="20">
         <v>2</v>
       </c>
       <c r="J30" s="15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K30" s="40" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L30" s="40" t="s">
+        <v>225</v>
+      </c>
+      <c r="M30" s="41" t="s">
+        <v>226</v>
+      </c>
+      <c r="N30" s="40" t="s">
         <v>227</v>
-      </c>
-      <c r="M30" s="41" t="s">
-        <v>228</v>
-      </c>
-      <c r="N30" s="40" t="s">
-        <v>229</v>
       </c>
       <c r="O30" s="20"/>
       <c r="P30" s="20"/>
       <c r="Q30" s="20"/>
       <c r="R30" s="20" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="S30" s="30" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="T30" s="20" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="U30" s="15" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="V30" s="20"/>
       <c r="W30" s="20"/>
@@ -4772,10 +4781,10 @@
       <c r="Y30" s="20"/>
       <c r="Z30" s="20"/>
       <c r="AA30" s="20" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AB30" s="16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AC30" s="20"/>
       <c r="AD30" s="20"/>
@@ -4784,10 +4793,10 @@
       <c r="AG30" s="20"/>
       <c r="AH30" s="20"/>
       <c r="AI30" s="20" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="AJ30" s="20" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="AK30" s="18" t="s">
         <v>106</v>
@@ -4804,10 +4813,10 @@
     </row>
     <row r="31" spans="1:46" ht="19.5" customHeight="1">
       <c r="A31" s="20" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C31" s="20" t="s">
         <v>115</v>
@@ -4822,43 +4831,43 @@
         <v>1</v>
       </c>
       <c r="G31" s="15" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H31" s="20" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I31" s="20">
         <v>2</v>
       </c>
       <c r="J31" s="15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K31" s="45" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="L31" s="45" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="M31" s="46" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="N31" s="45" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="O31" s="20"/>
       <c r="P31" s="20"/>
       <c r="Q31" s="20"/>
       <c r="R31" s="20" t="s">
+        <v>342</v>
+      </c>
+      <c r="S31" s="30" t="s">
+        <v>346</v>
+      </c>
+      <c r="T31" s="20" t="s">
+        <v>345</v>
+      </c>
+      <c r="U31" s="15" t="s">
         <v>344</v>
-      </c>
-      <c r="S31" s="30" t="s">
-        <v>348</v>
-      </c>
-      <c r="T31" s="20" t="s">
-        <v>347</v>
-      </c>
-      <c r="U31" s="15" t="s">
-        <v>346</v>
       </c>
       <c r="V31" s="20"/>
       <c r="W31" s="20"/>
@@ -4866,10 +4875,10 @@
       <c r="Y31" s="20"/>
       <c r="Z31" s="20"/>
       <c r="AA31" s="20" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AB31" s="16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AC31" s="20"/>
       <c r="AD31" s="20"/>
@@ -4878,10 +4887,10 @@
       <c r="AG31" s="20"/>
       <c r="AH31" s="20"/>
       <c r="AI31" s="20" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="AJ31" s="20" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="AK31" s="18" t="s">
         <v>106</v>
@@ -4898,10 +4907,10 @@
     </row>
     <row r="32" spans="1:46" ht="19.5" customHeight="1">
       <c r="A32" s="20" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C32" s="20" t="s">
         <v>115</v>
@@ -4916,43 +4925,43 @@
         <v>1</v>
       </c>
       <c r="G32" s="15" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H32" s="20" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I32" s="20">
         <v>2</v>
       </c>
       <c r="J32" s="15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K32" s="45" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="L32" s="45" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="M32" s="46" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="N32" s="45" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="O32" s="20"/>
       <c r="P32" s="20"/>
       <c r="Q32" s="20"/>
       <c r="R32" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="S32" s="30" t="s">
+        <v>346</v>
+      </c>
+      <c r="T32" s="20" t="s">
         <v>345</v>
       </c>
-      <c r="S32" s="30" t="s">
-        <v>348</v>
-      </c>
-      <c r="T32" s="20" t="s">
-        <v>347</v>
-      </c>
       <c r="U32" s="15" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="V32" s="20"/>
       <c r="W32" s="20"/>
@@ -4960,10 +4969,10 @@
       <c r="Y32" s="20"/>
       <c r="Z32" s="20"/>
       <c r="AA32" s="20" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AB32" s="16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AC32" s="20"/>
       <c r="AD32" s="20"/>
@@ -4972,10 +4981,10 @@
       <c r="AG32" s="20"/>
       <c r="AH32" s="20"/>
       <c r="AI32" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="AJ32" s="20" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="AK32" s="20"/>
       <c r="AL32" s="20"/>
@@ -4990,10 +4999,10 @@
     </row>
     <row r="33" spans="1:46" ht="19.5" customHeight="1">
       <c r="A33" s="20" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C33" s="20" t="s">
         <v>115</v>
@@ -5008,28 +5017,28 @@
         <v>1</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H33" s="20" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="I33" s="20">
         <v>2</v>
       </c>
       <c r="J33" s="15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K33" s="45" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L33" s="45" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="M33" s="46" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="N33" s="45" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="O33" s="20"/>
       <c r="P33" s="20"/>
@@ -5044,10 +5053,10 @@
       <c r="Y33" s="20"/>
       <c r="Z33" s="20"/>
       <c r="AA33" s="20" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AB33" s="16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AC33" s="20"/>
       <c r="AD33" s="20"/>
@@ -5070,10 +5079,10 @@
     </row>
     <row r="34" spans="1:46" ht="19.5" customHeight="1">
       <c r="A34" s="20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C34" s="20" t="s">
         <v>115</v>
@@ -5088,28 +5097,28 @@
         <v>1</v>
       </c>
       <c r="G34" s="15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H34" s="20" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I34" s="20">
         <v>2</v>
       </c>
       <c r="J34" s="15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K34" s="45" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="L34" s="45" t="s">
+        <v>234</v>
+      </c>
+      <c r="M34" s="46" t="s">
+        <v>235</v>
+      </c>
+      <c r="N34" s="45" t="s">
         <v>236</v>
-      </c>
-      <c r="M34" s="46" t="s">
-        <v>237</v>
-      </c>
-      <c r="N34" s="45" t="s">
-        <v>238</v>
       </c>
       <c r="O34" s="20"/>
       <c r="P34" s="20"/>
@@ -5124,10 +5133,10 @@
       <c r="Y34" s="20"/>
       <c r="Z34" s="20"/>
       <c r="AA34" s="20" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AB34" s="16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AC34" s="20"/>
       <c r="AD34" s="20"/>
@@ -5150,46 +5159,38 @@
     </row>
     <row r="35" spans="1:46" ht="19.5" customHeight="1">
       <c r="A35" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>349</v>
+      </c>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="B35" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="C35" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="D35" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="E35" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="F35" s="20">
-        <v>1</v>
-      </c>
-      <c r="G35" s="15" t="s">
-        <v>162</v>
-      </c>
       <c r="H35" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I35" s="20">
         <v>2</v>
       </c>
       <c r="J35" s="15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K35" s="45" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="L35" s="45" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="M35" s="46" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="N35" s="45" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="O35" s="20"/>
       <c r="P35" s="20"/>
@@ -5204,10 +5205,10 @@
       <c r="Y35" s="20"/>
       <c r="Z35" s="20"/>
       <c r="AA35" s="20" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AB35" s="16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AC35" s="20"/>
       <c r="AD35" s="20"/>
@@ -5230,46 +5231,38 @@
     </row>
     <row r="36" spans="1:46" ht="19.5" customHeight="1">
       <c r="A36" s="20" t="s">
+        <v>350</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>351</v>
+      </c>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="B36" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="C36" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="E36" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="F36" s="20">
-        <v>1</v>
-      </c>
-      <c r="G36" s="15" t="s">
-        <v>165</v>
-      </c>
       <c r="H36" s="20" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I36" s="20">
         <v>2</v>
       </c>
       <c r="J36" s="15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K36" s="45" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="L36" s="45" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="M36" s="46" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="N36" s="45" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="O36" s="20"/>
       <c r="P36" s="20"/>
@@ -5284,10 +5277,10 @@
       <c r="Y36" s="20"/>
       <c r="Z36" s="20"/>
       <c r="AA36" s="20" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AB36" s="16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AC36" s="20"/>
       <c r="AD36" s="20"/>
@@ -5310,13 +5303,13 @@
     </row>
     <row r="37" spans="1:46" ht="19.5" customHeight="1">
       <c r="A37" s="20" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="D37" s="20" t="s">
         <v>130</v>
@@ -5328,28 +5321,28 @@
         <v>1</v>
       </c>
       <c r="G37" s="15" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H37" s="20" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I37" s="20">
         <v>2</v>
       </c>
       <c r="J37" s="15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K37" s="45" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="L37" s="45" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M37" s="46" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="N37" s="45" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="O37" s="20"/>
       <c r="P37" s="20"/>
@@ -5364,10 +5357,10 @@
       <c r="Y37" s="20"/>
       <c r="Z37" s="20"/>
       <c r="AA37" s="20" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AB37" s="16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AC37" s="20"/>
       <c r="AD37" s="20"/>
@@ -5390,13 +5383,13 @@
     </row>
     <row r="38" spans="1:46" ht="19.5" customHeight="1">
       <c r="A38" s="20" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="C38" s="27" t="s">
-        <v>115</v>
+        <v>162</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>95</v>
       </c>
       <c r="D38" s="20" t="s">
         <v>130</v>
@@ -5408,28 +5401,28 @@
         <v>1</v>
       </c>
       <c r="G38" s="15" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H38" s="20" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I38" s="20">
         <v>2</v>
       </c>
       <c r="J38" s="15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K38" s="45" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="L38" s="45" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="M38" s="46" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="N38" s="45" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="O38" s="20"/>
       <c r="P38" s="20"/>
@@ -5444,10 +5437,10 @@
       <c r="Y38" s="20"/>
       <c r="Z38" s="20"/>
       <c r="AA38" s="20" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AB38" s="16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AC38" s="20"/>
       <c r="AD38" s="20"/>
@@ -5470,10 +5463,10 @@
     </row>
     <row r="39" spans="1:46" ht="19.5" customHeight="1">
       <c r="A39" s="20" t="s">
-        <v>199</v>
+        <v>163</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C39" s="20" t="s">
         <v>115</v>
@@ -5488,28 +5481,28 @@
         <v>1</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="H39" s="20" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I39" s="20">
         <v>2</v>
       </c>
       <c r="J39" s="15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K39" s="45" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="L39" s="45" t="s">
+        <v>245</v>
+      </c>
+      <c r="M39" s="46" t="s">
+        <v>246</v>
+      </c>
+      <c r="N39" s="45" t="s">
         <v>247</v>
-      </c>
-      <c r="M39" s="46" t="s">
-        <v>248</v>
-      </c>
-      <c r="N39" s="45" t="s">
-        <v>249</v>
       </c>
       <c r="O39" s="20"/>
       <c r="P39" s="20"/>
@@ -5524,10 +5517,10 @@
       <c r="Y39" s="20"/>
       <c r="Z39" s="20"/>
       <c r="AA39" s="20" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AB39" s="16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AC39" s="20"/>
       <c r="AD39" s="20"/>
@@ -5549,47 +5542,47 @@
       <c r="AT39" s="2"/>
     </row>
     <row r="40" spans="1:46" ht="19.5" customHeight="1">
-      <c r="A40" s="28" t="s">
-        <v>200</v>
-      </c>
-      <c r="B40" s="28" t="s">
-        <v>170</v>
-      </c>
-      <c r="C40" s="28" t="s">
+      <c r="A40" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="C40" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="D40" s="28" t="s">
+      <c r="D40" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="E40" s="28" t="s">
+      <c r="E40" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="F40" s="28">
+      <c r="F40" s="20">
         <v>1</v>
       </c>
       <c r="G40" s="31" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H40" s="35" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I40" s="28">
         <v>2</v>
       </c>
       <c r="J40" s="15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K40" s="42" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="L40" s="42" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="M40" s="43" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="N40" s="42" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="O40" s="28"/>
       <c r="P40" s="28"/>
@@ -5604,10 +5597,10 @@
       <c r="Y40" s="28"/>
       <c r="Z40" s="28"/>
       <c r="AA40" s="28" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AB40" s="16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AC40" s="28"/>
       <c r="AD40" s="28"/>
@@ -5629,27 +5622,39 @@
       <c r="AT40" s="2"/>
     </row>
     <row r="41" spans="1:46" ht="19.5" customHeight="1">
-      <c r="A41" s="32"/>
-      <c r="B41" s="32"/>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="33"/>
+      <c r="A41" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="F41" s="20">
+        <v>1</v>
+      </c>
       <c r="G41" s="33"/>
       <c r="H41" s="33"/>
       <c r="I41" s="33"/>
       <c r="J41" s="33"/>
       <c r="K41" s="39" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="L41" s="39" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="M41" s="44" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="N41" s="39" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="O41" s="33"/>
       <c r="P41" s="33"/>
@@ -5664,10 +5669,10 @@
       <c r="Y41" s="33"/>
       <c r="Z41" s="33"/>
       <c r="AA41" s="33" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AB41" s="16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AC41" s="33"/>
       <c r="AD41" s="33"/>
@@ -5689,27 +5694,39 @@
       <c r="AT41" s="2"/>
     </row>
     <row r="42" spans="1:46" ht="12.75" customHeight="1">
-      <c r="A42" s="32"/>
-      <c r="B42" s="32"/>
-      <c r="C42" s="32"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="32"/>
-      <c r="F42" s="33"/>
+      <c r="A42" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="B42" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="C42" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="D42" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="E42" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="F42" s="28">
+        <v>1</v>
+      </c>
       <c r="G42" s="33"/>
       <c r="H42" s="33"/>
       <c r="I42" s="33"/>
       <c r="J42" s="33"/>
       <c r="K42" s="39" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="L42" s="39" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="M42" s="39" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="N42" s="39" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="O42" s="33"/>
       <c r="P42" s="33"/>
@@ -5724,10 +5741,10 @@
       <c r="Y42" s="33"/>
       <c r="Z42" s="33"/>
       <c r="AA42" s="33" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AB42" s="16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AC42" s="33"/>
       <c r="AD42" s="33"/>
@@ -5749,27 +5766,27 @@
       <c r="AT42" s="2"/>
     </row>
     <row r="43" spans="1:46" ht="12.75" customHeight="1">
-      <c r="A43" s="34"/>
-      <c r="B43" s="34"/>
-      <c r="C43" s="34"/>
-      <c r="D43" s="34"/>
-      <c r="E43" s="34"/>
-      <c r="F43" s="32"/>
+      <c r="A43" s="32"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="33"/>
       <c r="G43" s="33"/>
       <c r="H43" s="33"/>
       <c r="I43" s="32"/>
       <c r="J43" s="32"/>
       <c r="K43" s="39" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="L43" s="39" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="M43" s="39" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="N43" s="39" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="O43" s="32"/>
       <c r="P43" s="32"/>
@@ -5784,10 +5801,10 @@
       <c r="Y43" s="32"/>
       <c r="Z43" s="32"/>
       <c r="AA43" s="32" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AB43" s="16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AC43" s="32"/>
       <c r="AD43" s="32"/>
@@ -5809,27 +5826,27 @@
       <c r="AT43" s="2"/>
     </row>
     <row r="44" spans="1:46" ht="12.75" customHeight="1">
-      <c r="A44" s="34"/>
-      <c r="B44" s="34"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="34"/>
-      <c r="E44" s="34"/>
-      <c r="F44" s="32"/>
+      <c r="A44" s="32"/>
+      <c r="B44" s="32"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="32"/>
+      <c r="E44" s="32"/>
+      <c r="F44" s="33"/>
       <c r="G44" s="33"/>
       <c r="H44" s="33"/>
       <c r="I44" s="32"/>
       <c r="J44" s="32"/>
       <c r="K44" s="39" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="L44" s="39" t="s">
+        <v>256</v>
+      </c>
+      <c r="M44" s="39" t="s">
+        <v>257</v>
+      </c>
+      <c r="N44" s="39" t="s">
         <v>258</v>
-      </c>
-      <c r="M44" s="39" t="s">
-        <v>259</v>
-      </c>
-      <c r="N44" s="39" t="s">
-        <v>260</v>
       </c>
       <c r="O44" s="32"/>
       <c r="P44" s="32"/>
@@ -5844,10 +5861,10 @@
       <c r="Y44" s="32"/>
       <c r="Z44" s="32"/>
       <c r="AA44" s="32" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="AB44" s="16" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AC44" s="32"/>
       <c r="AD44" s="32"/>
@@ -5970,7 +5987,7 @@
       <c r="C47" s="34"/>
       <c r="D47" s="34"/>
       <c r="E47" s="34"/>
-      <c r="F47" s="34"/>
+      <c r="F47" s="32"/>
       <c r="G47" s="32"/>
       <c r="H47" s="32"/>
       <c r="I47" s="34"/>
@@ -6008,6 +6025,12 @@
       <c r="AO47" s="34"/>
     </row>
     <row r="48" spans="1:46" ht="12.75" customHeight="1">
+      <c r="A48" s="34"/>
+      <c r="B48" s="34"/>
+      <c r="C48" s="34"/>
+      <c r="D48" s="34"/>
+      <c r="E48" s="34"/>
+      <c r="F48" s="32"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
@@ -6050,14 +6073,12 @@
       <c r="AT48" s="2"/>
     </row>
     <row r="49" spans="1:46" ht="12.75" customHeight="1">
-      <c r="A49" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="B49" s="9"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
+      <c r="A49" s="34"/>
+      <c r="B49" s="34"/>
+      <c r="C49" s="34"/>
+      <c r="D49" s="34"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="34"/>
       <c r="G49" s="9"/>
       <c r="H49" s="9"/>
       <c r="I49" s="9"/>
@@ -6100,14 +6121,6 @@
       <c r="AT49" s="9"/>
     </row>
     <row r="50" spans="1:46" ht="12.75" customHeight="1">
-      <c r="A50" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
@@ -6150,14 +6163,14 @@
       <c r="AT50" s="2"/>
     </row>
     <row r="51" spans="1:46" ht="12.75" customHeight="1">
-      <c r="A51" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
+      <c r="A51" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
@@ -6201,7 +6214,7 @@
     </row>
     <row r="52" spans="1:46" ht="12.75" customHeight="1">
       <c r="A52" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -6251,12 +6264,12 @@
     </row>
     <row r="53" spans="1:46" ht="12.75" customHeight="1">
       <c r="A53" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
-      <c r="E53" s="4"/>
+      <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
@@ -6301,12 +6314,12 @@
     </row>
     <row r="54" spans="1:46" ht="12.75" customHeight="1">
       <c r="A54" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
-      <c r="E54" s="4"/>
+      <c r="E54" s="2"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
@@ -6350,15 +6363,13 @@
       <c r="AT54" s="2"/>
     </row>
     <row r="55" spans="1:46" ht="12.75" customHeight="1">
-      <c r="A55" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="B55" s="22"/>
-      <c r="C55" s="22"/>
-      <c r="D55" s="22"/>
-      <c r="E55" s="22" t="s">
-        <v>70</v>
-      </c>
+      <c r="A55" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="4"/>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
@@ -6402,12 +6413,14 @@
       <c r="AT55" s="2"/>
     </row>
     <row r="56" spans="1:46" ht="12.75" customHeight="1">
-      <c r="A56" s="22"/>
-      <c r="B56" s="22"/>
-      <c r="C56" s="22"/>
-      <c r="D56" s="22"/>
-      <c r="E56" s="22"/>
-      <c r="F56" s="22"/>
+      <c r="A56" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="2"/>
       <c r="G56" s="22"/>
       <c r="H56" s="22"/>
       <c r="I56" s="2"/>
@@ -6450,16 +6463,16 @@
       <c r="AT56" s="2"/>
     </row>
     <row r="57" spans="1:46" ht="21" customHeight="1">
-      <c r="A57" s="24" t="s">
-        <v>119</v>
+      <c r="A57" s="22" t="s">
+        <v>69</v>
       </c>
       <c r="B57" s="22"/>
       <c r="C57" s="22"/>
       <c r="D57" s="22"/>
-      <c r="E57" s="25">
-        <v>45347</v>
-      </c>
-      <c r="F57" s="22"/>
+      <c r="E57" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="F57" s="2"/>
       <c r="G57" s="22"/>
       <c r="H57" s="22"/>
       <c r="I57" s="2"/>
@@ -6502,11 +6515,11 @@
       <c r="AT57" s="2"/>
     </row>
     <row r="58" spans="1:46" ht="12.75" customHeight="1">
-      <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
+      <c r="A58" s="22"/>
+      <c r="B58" s="22"/>
+      <c r="C58" s="22"/>
+      <c r="D58" s="22"/>
+      <c r="E58" s="22"/>
       <c r="F58" s="22"/>
       <c r="G58" s="22"/>
       <c r="H58" s="22"/>
@@ -6550,11 +6563,15 @@
       <c r="AT58" s="2"/>
     </row>
     <row r="59" spans="1:46" ht="12.75" customHeight="1">
-      <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
+      <c r="A59" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="B59" s="22"/>
+      <c r="C59" s="22"/>
+      <c r="D59" s="22"/>
+      <c r="E59" s="25">
+        <v>45347</v>
+      </c>
       <c r="F59" s="22"/>
       <c r="G59" s="22"/>
       <c r="H59" s="22"/>
@@ -6603,7 +6620,7 @@
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
+      <c r="F60" s="22"/>
       <c r="G60" s="22"/>
       <c r="H60" s="22"/>
       <c r="I60" s="2"/>
@@ -6651,7 +6668,7 @@
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
+      <c r="F61" s="22"/>
       <c r="G61" s="22"/>
       <c r="H61" s="22"/>
       <c r="I61" s="2"/>
@@ -16102,6 +16119,11 @@
       <c r="AT257" s="2"/>
     </row>
     <row r="258" spans="1:46" ht="12.75" customHeight="1">
+      <c r="A258" s="2"/>
+      <c r="B258" s="2"/>
+      <c r="C258" s="2"/>
+      <c r="D258" s="2"/>
+      <c r="E258" s="2"/>
       <c r="F258" s="2"/>
       <c r="G258" s="2"/>
       <c r="H258" s="2"/>
@@ -16145,6 +16167,11 @@
       <c r="AT258" s="2"/>
     </row>
     <row r="259" spans="1:46" ht="12.75" customHeight="1">
+      <c r="A259" s="2"/>
+      <c r="B259" s="2"/>
+      <c r="C259" s="2"/>
+      <c r="D259" s="2"/>
+      <c r="E259" s="2"/>
       <c r="F259" s="2"/>
       <c r="G259" s="2"/>
       <c r="H259" s="2"/>
@@ -16188,10 +16215,12 @@
       <c r="AT259" s="2"/>
     </row>
     <row r="260" spans="1:46" ht="15.75" customHeight="1">
+      <c r="F260" s="2"/>
       <c r="G260" s="2"/>
       <c r="H260" s="2"/>
     </row>
     <row r="261" spans="1:46" ht="15.75" customHeight="1">
+      <c r="F261" s="2"/>
       <c r="G261" s="2"/>
       <c r="H261" s="2"/>
     </row>
@@ -16955,16 +16984,6 @@
     <row r="1019" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="Z18:AB18"/>
-    <mergeCell ref="AC18:AE18"/>
-    <mergeCell ref="AF18:AH18"/>
-    <mergeCell ref="B4:Q4"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="D8:J8"/>
-    <mergeCell ref="D9:J9"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B6:E6"/>
     <mergeCell ref="AN15:AO18"/>
     <mergeCell ref="W17:Y17"/>
     <mergeCell ref="Z17:AB17"/>
@@ -16981,6 +17000,16 @@
     <mergeCell ref="AF15:AM17"/>
     <mergeCell ref="R18:V18"/>
     <mergeCell ref="W18:Y18"/>
+    <mergeCell ref="Z18:AB18"/>
+    <mergeCell ref="AC18:AE18"/>
+    <mergeCell ref="AF18:AH18"/>
+    <mergeCell ref="B4:Q4"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="D8:J8"/>
+    <mergeCell ref="D9:J9"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B6:E6"/>
   </mergeCells>
   <phoneticPr fontId="21" type="noConversion"/>
   <hyperlinks>
@@ -17117,17 +17146,17 @@
       <c r="V3" s="2"/>
     </row>
     <row r="4" spans="1:46" ht="12.75" customHeight="1">
-      <c r="A4" s="81" t="s">
+      <c r="A4" s="84" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
@@ -17617,57 +17646,57 @@
       <c r="AT14" s="9"/>
     </row>
     <row r="15" spans="1:46" ht="12.75" customHeight="1">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="68" t="s">
+      <c r="B15" s="69"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="59"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="59"/>
-      <c r="N15" s="59"/>
-      <c r="O15" s="59"/>
-      <c r="P15" s="59"/>
-      <c r="Q15" s="59"/>
-      <c r="R15" s="59"/>
-      <c r="S15" s="59"/>
-      <c r="T15" s="59"/>
-      <c r="U15" s="59"/>
-      <c r="V15" s="48"/>
-      <c r="W15" s="69" t="s">
+      <c r="H15" s="69"/>
+      <c r="I15" s="69"/>
+      <c r="J15" s="69"/>
+      <c r="K15" s="69"/>
+      <c r="L15" s="69"/>
+      <c r="M15" s="69"/>
+      <c r="N15" s="69"/>
+      <c r="O15" s="69"/>
+      <c r="P15" s="69"/>
+      <c r="Q15" s="69"/>
+      <c r="R15" s="69"/>
+      <c r="S15" s="69"/>
+      <c r="T15" s="69"/>
+      <c r="U15" s="69"/>
+      <c r="V15" s="60"/>
+      <c r="W15" s="78" t="s">
         <v>78</v>
       </c>
-      <c r="X15" s="59"/>
-      <c r="Y15" s="59"/>
-      <c r="Z15" s="59"/>
-      <c r="AA15" s="59"/>
-      <c r="AB15" s="59"/>
-      <c r="AC15" s="59"/>
-      <c r="AD15" s="59"/>
-      <c r="AE15" s="48"/>
-      <c r="AF15" s="70" t="s">
+      <c r="X15" s="69"/>
+      <c r="Y15" s="69"/>
+      <c r="Z15" s="69"/>
+      <c r="AA15" s="69"/>
+      <c r="AB15" s="69"/>
+      <c r="AC15" s="69"/>
+      <c r="AD15" s="69"/>
+      <c r="AE15" s="60"/>
+      <c r="AF15" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="AG15" s="59"/>
-      <c r="AH15" s="59"/>
-      <c r="AI15" s="59"/>
-      <c r="AJ15" s="59"/>
-      <c r="AK15" s="59"/>
-      <c r="AL15" s="59"/>
-      <c r="AM15" s="48"/>
-      <c r="AN15" s="47" t="s">
+      <c r="AG15" s="69"/>
+      <c r="AH15" s="69"/>
+      <c r="AI15" s="69"/>
+      <c r="AJ15" s="69"/>
+      <c r="AK15" s="69"/>
+      <c r="AL15" s="69"/>
+      <c r="AM15" s="60"/>
+      <c r="AN15" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="AO15" s="48"/>
+      <c r="AO15" s="60"/>
       <c r="AP15" s="10"/>
       <c r="AQ15" s="10"/>
       <c r="AR15" s="10"/>
@@ -17675,47 +17704,47 @@
       <c r="AT15" s="10"/>
     </row>
     <row r="16" spans="1:46" ht="12.75" customHeight="1">
-      <c r="A16" s="49"/>
-      <c r="B16" s="60"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="60"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="60"/>
-      <c r="J16" s="60"/>
-      <c r="K16" s="60"/>
-      <c r="L16" s="60"/>
-      <c r="M16" s="60"/>
-      <c r="N16" s="60"/>
-      <c r="O16" s="60"/>
-      <c r="P16" s="60"/>
-      <c r="Q16" s="60"/>
-      <c r="R16" s="60"/>
-      <c r="S16" s="60"/>
-      <c r="T16" s="60"/>
-      <c r="U16" s="60"/>
-      <c r="V16" s="50"/>
-      <c r="W16" s="51"/>
-      <c r="X16" s="61"/>
-      <c r="Y16" s="61"/>
-      <c r="Z16" s="61"/>
-      <c r="AA16" s="61"/>
-      <c r="AB16" s="61"/>
-      <c r="AC16" s="61"/>
-      <c r="AD16" s="61"/>
-      <c r="AE16" s="52"/>
-      <c r="AF16" s="49"/>
-      <c r="AG16" s="60"/>
-      <c r="AH16" s="60"/>
-      <c r="AI16" s="60"/>
-      <c r="AJ16" s="60"/>
-      <c r="AK16" s="60"/>
-      <c r="AL16" s="60"/>
-      <c r="AM16" s="50"/>
-      <c r="AN16" s="49"/>
-      <c r="AO16" s="50"/>
+      <c r="A16" s="61"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="70"/>
+      <c r="F16" s="62"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="70"/>
+      <c r="I16" s="70"/>
+      <c r="J16" s="70"/>
+      <c r="K16" s="70"/>
+      <c r="L16" s="70"/>
+      <c r="M16" s="70"/>
+      <c r="N16" s="70"/>
+      <c r="O16" s="70"/>
+      <c r="P16" s="70"/>
+      <c r="Q16" s="70"/>
+      <c r="R16" s="70"/>
+      <c r="S16" s="70"/>
+      <c r="T16" s="70"/>
+      <c r="U16" s="70"/>
+      <c r="V16" s="62"/>
+      <c r="W16" s="63"/>
+      <c r="X16" s="71"/>
+      <c r="Y16" s="71"/>
+      <c r="Z16" s="71"/>
+      <c r="AA16" s="71"/>
+      <c r="AB16" s="71"/>
+      <c r="AC16" s="71"/>
+      <c r="AD16" s="71"/>
+      <c r="AE16" s="64"/>
+      <c r="AF16" s="61"/>
+      <c r="AG16" s="70"/>
+      <c r="AH16" s="70"/>
+      <c r="AI16" s="70"/>
+      <c r="AJ16" s="70"/>
+      <c r="AK16" s="70"/>
+      <c r="AL16" s="70"/>
+      <c r="AM16" s="62"/>
+      <c r="AN16" s="61"/>
+      <c r="AO16" s="62"/>
       <c r="AP16" s="10"/>
       <c r="AQ16" s="10"/>
       <c r="AR16" s="10"/>
@@ -17723,53 +17752,53 @@
       <c r="AT16" s="10"/>
     </row>
     <row r="17" spans="1:46" ht="26.25" customHeight="1">
-      <c r="A17" s="51"/>
-      <c r="B17" s="61"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="61"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="61"/>
-      <c r="L17" s="61"/>
-      <c r="M17" s="61"/>
-      <c r="N17" s="61"/>
-      <c r="O17" s="61"/>
-      <c r="P17" s="61"/>
-      <c r="Q17" s="61"/>
-      <c r="R17" s="61"/>
-      <c r="S17" s="61"/>
-      <c r="T17" s="61"/>
-      <c r="U17" s="61"/>
-      <c r="V17" s="52"/>
-      <c r="W17" s="53" t="s">
+      <c r="A17" s="63"/>
+      <c r="B17" s="71"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="71"/>
+      <c r="E17" s="71"/>
+      <c r="F17" s="64"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="71"/>
+      <c r="J17" s="71"/>
+      <c r="K17" s="71"/>
+      <c r="L17" s="71"/>
+      <c r="M17" s="71"/>
+      <c r="N17" s="71"/>
+      <c r="O17" s="71"/>
+      <c r="P17" s="71"/>
+      <c r="Q17" s="71"/>
+      <c r="R17" s="71"/>
+      <c r="S17" s="71"/>
+      <c r="T17" s="71"/>
+      <c r="U17" s="71"/>
+      <c r="V17" s="64"/>
+      <c r="W17" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="X17" s="54"/>
-      <c r="Y17" s="55"/>
-      <c r="Z17" s="56" t="s">
+      <c r="X17" s="48"/>
+      <c r="Y17" s="49"/>
+      <c r="Z17" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="AA17" s="54"/>
-      <c r="AB17" s="55"/>
-      <c r="AC17" s="57" t="s">
+      <c r="AA17" s="48"/>
+      <c r="AB17" s="49"/>
+      <c r="AC17" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="AD17" s="54"/>
-      <c r="AE17" s="55"/>
-      <c r="AF17" s="51"/>
-      <c r="AG17" s="61"/>
-      <c r="AH17" s="61"/>
-      <c r="AI17" s="61"/>
-      <c r="AJ17" s="61"/>
-      <c r="AK17" s="61"/>
-      <c r="AL17" s="61"/>
-      <c r="AM17" s="52"/>
-      <c r="AN17" s="49"/>
-      <c r="AO17" s="50"/>
+      <c r="AD17" s="48"/>
+      <c r="AE17" s="49"/>
+      <c r="AF17" s="63"/>
+      <c r="AG17" s="71"/>
+      <c r="AH17" s="71"/>
+      <c r="AI17" s="71"/>
+      <c r="AJ17" s="71"/>
+      <c r="AK17" s="71"/>
+      <c r="AL17" s="71"/>
+      <c r="AM17" s="64"/>
+      <c r="AN17" s="61"/>
+      <c r="AO17" s="62"/>
       <c r="AP17" s="10"/>
       <c r="AQ17" s="10"/>
       <c r="AR17" s="10"/>
@@ -17777,69 +17806,69 @@
       <c r="AT17" s="10"/>
     </row>
     <row r="18" spans="1:46">
-      <c r="A18" s="62" t="s">
+      <c r="A18" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="54"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="63" t="s">
+      <c r="B18" s="48"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="49"/>
+      <c r="G18" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="64" t="s">
+      <c r="H18" s="48"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="L18" s="54"/>
-      <c r="M18" s="54"/>
-      <c r="N18" s="55"/>
-      <c r="O18" s="65" t="s">
+      <c r="L18" s="48"/>
+      <c r="M18" s="48"/>
+      <c r="N18" s="49"/>
+      <c r="O18" s="75" t="s">
         <v>80</v>
       </c>
-      <c r="P18" s="54"/>
-      <c r="Q18" s="55"/>
-      <c r="R18" s="71" t="s">
+      <c r="P18" s="48"/>
+      <c r="Q18" s="49"/>
+      <c r="R18" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="S18" s="54"/>
-      <c r="T18" s="54"/>
-      <c r="U18" s="54"/>
-      <c r="V18" s="55"/>
-      <c r="W18" s="72" t="s">
+      <c r="S18" s="48"/>
+      <c r="T18" s="48"/>
+      <c r="U18" s="48"/>
+      <c r="V18" s="49"/>
+      <c r="W18" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="X18" s="54"/>
-      <c r="Y18" s="55"/>
-      <c r="Z18" s="72" t="s">
+      <c r="X18" s="48"/>
+      <c r="Y18" s="49"/>
+      <c r="Z18" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="AA18" s="54"/>
-      <c r="AB18" s="55"/>
-      <c r="AC18" s="72" t="s">
+      <c r="AA18" s="48"/>
+      <c r="AB18" s="49"/>
+      <c r="AC18" s="47" t="s">
         <v>83</v>
       </c>
-      <c r="AD18" s="54"/>
-      <c r="AE18" s="55"/>
-      <c r="AF18" s="66" t="s">
+      <c r="AD18" s="48"/>
+      <c r="AE18" s="49"/>
+      <c r="AF18" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="AG18" s="54"/>
-      <c r="AH18" s="55"/>
-      <c r="AI18" s="66" t="s">
+      <c r="AG18" s="48"/>
+      <c r="AH18" s="49"/>
+      <c r="AI18" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="AJ18" s="54"/>
-      <c r="AK18" s="55"/>
-      <c r="AL18" s="67" t="s">
+      <c r="AJ18" s="48"/>
+      <c r="AK18" s="49"/>
+      <c r="AL18" s="76" t="s">
         <v>85</v>
       </c>
-      <c r="AM18" s="52"/>
-      <c r="AN18" s="51"/>
-      <c r="AO18" s="52"/>
+      <c r="AM18" s="64"/>
+      <c r="AN18" s="63"/>
+      <c r="AO18" s="64"/>
       <c r="AP18" s="10"/>
       <c r="AQ18" s="10"/>
       <c r="AR18" s="10"/>
@@ -18065,55 +18094,55 @@
       <c r="AT20" s="19"/>
     </row>
     <row r="21" spans="1:46" ht="12.75" customHeight="1">
-      <c r="A21" s="82" t="s">
+      <c r="A21" s="81" t="s">
         <v>93</v>
       </c>
-      <c r="B21" s="82" t="s">
+      <c r="B21" s="81" t="s">
         <v>94</v>
       </c>
-      <c r="C21" s="82" t="s">
+      <c r="C21" s="81" t="s">
         <v>95</v>
       </c>
-      <c r="D21" s="82" t="s">
+      <c r="D21" s="81" t="s">
         <v>96</v>
       </c>
-      <c r="E21" s="85">
+      <c r="E21" s="86">
         <v>44650</v>
       </c>
-      <c r="F21" s="82">
+      <c r="F21" s="81">
         <v>1</v>
       </c>
-      <c r="G21" s="82" t="s">
+      <c r="G21" s="81" t="s">
         <v>97</v>
       </c>
-      <c r="H21" s="82" t="s">
+      <c r="H21" s="81" t="s">
         <v>98</v>
       </c>
-      <c r="I21" s="82" t="s">
+      <c r="I21" s="81" t="s">
         <v>99</v>
       </c>
-      <c r="J21" s="82">
+      <c r="J21" s="81">
         <v>1</v>
       </c>
-      <c r="K21" s="86" t="s">
+      <c r="K21" s="83" t="s">
         <v>100</v>
       </c>
-      <c r="L21" s="82" t="s">
+      <c r="L21" s="81" t="s">
         <v>101</v>
       </c>
-      <c r="M21" s="82" t="s">
+      <c r="M21" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="N21" s="82" t="s">
+      <c r="N21" s="81" t="s">
         <v>103</v>
       </c>
-      <c r="O21" s="82" t="s">
+      <c r="O21" s="81" t="s">
         <v>104</v>
       </c>
-      <c r="P21" s="82" t="s">
+      <c r="P21" s="81" t="s">
         <v>105</v>
       </c>
-      <c r="Q21" s="82" t="s">
+      <c r="Q21" s="81" t="s">
         <v>106</v>
       </c>
       <c r="R21" s="20" t="s">
@@ -18159,23 +18188,23 @@
       <c r="AT21" s="2"/>
     </row>
     <row r="22" spans="1:46" ht="12.75" customHeight="1">
-      <c r="A22" s="84"/>
-      <c r="B22" s="84"/>
-      <c r="C22" s="84"/>
-      <c r="D22" s="84"/>
-      <c r="E22" s="84"/>
-      <c r="F22" s="84"/>
-      <c r="G22" s="83"/>
-      <c r="H22" s="83"/>
-      <c r="I22" s="83"/>
-      <c r="J22" s="83"/>
-      <c r="K22" s="52"/>
-      <c r="L22" s="83"/>
-      <c r="M22" s="83"/>
-      <c r="N22" s="83"/>
-      <c r="O22" s="83"/>
-      <c r="P22" s="83"/>
-      <c r="Q22" s="83"/>
+      <c r="A22" s="85"/>
+      <c r="B22" s="85"/>
+      <c r="C22" s="85"/>
+      <c r="D22" s="85"/>
+      <c r="E22" s="85"/>
+      <c r="F22" s="85"/>
+      <c r="G22" s="82"/>
+      <c r="H22" s="82"/>
+      <c r="I22" s="82"/>
+      <c r="J22" s="82"/>
+      <c r="K22" s="64"/>
+      <c r="L22" s="82"/>
+      <c r="M22" s="82"/>
+      <c r="N22" s="82"/>
+      <c r="O22" s="82"/>
+      <c r="P22" s="82"/>
+      <c r="Q22" s="82"/>
       <c r="R22" s="20" t="s">
         <v>113</v>
       </c>
@@ -18209,12 +18238,12 @@
       <c r="AT22" s="2"/>
     </row>
     <row r="23" spans="1:46" ht="12.75" customHeight="1">
-      <c r="A23" s="84"/>
-      <c r="B23" s="84"/>
-      <c r="C23" s="84"/>
-      <c r="D23" s="84"/>
-      <c r="E23" s="84"/>
-      <c r="F23" s="84"/>
+      <c r="A23" s="85"/>
+      <c r="B23" s="85"/>
+      <c r="C23" s="85"/>
+      <c r="D23" s="85"/>
+      <c r="E23" s="85"/>
+      <c r="F23" s="85"/>
       <c r="G23" s="20" t="s">
         <v>114</v>
       </c>
@@ -18265,12 +18294,12 @@
       <c r="AT23" s="2"/>
     </row>
     <row r="24" spans="1:46" ht="12.75" customHeight="1">
-      <c r="A24" s="83"/>
-      <c r="B24" s="83"/>
-      <c r="C24" s="83"/>
-      <c r="D24" s="83"/>
-      <c r="E24" s="83"/>
-      <c r="F24" s="83"/>
+      <c r="A24" s="82"/>
+      <c r="B24" s="82"/>
+      <c r="C24" s="82"/>
+      <c r="D24" s="82"/>
+      <c r="E24" s="82"/>
+      <c r="F24" s="82"/>
       <c r="G24" s="20" t="s">
         <v>117</v>
       </c>
@@ -29518,15 +29547,22 @@
     <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="P21:P22"/>
-    <mergeCell ref="Q21:Q22"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="L21:L22"/>
-    <mergeCell ref="M21:M22"/>
-    <mergeCell ref="N21:N22"/>
-    <mergeCell ref="O21:O22"/>
+    <mergeCell ref="AF15:AM17"/>
+    <mergeCell ref="AN15:AO18"/>
+    <mergeCell ref="W17:Y17"/>
+    <mergeCell ref="Z17:AB17"/>
+    <mergeCell ref="AC17:AE17"/>
+    <mergeCell ref="W18:Y18"/>
+    <mergeCell ref="Z18:AB18"/>
+    <mergeCell ref="AC18:AE18"/>
+    <mergeCell ref="AF18:AH18"/>
+    <mergeCell ref="AI18:AK18"/>
+    <mergeCell ref="AL18:AM18"/>
+    <mergeCell ref="K18:N18"/>
+    <mergeCell ref="O18:Q18"/>
+    <mergeCell ref="R18:V18"/>
+    <mergeCell ref="G15:V17"/>
+    <mergeCell ref="W15:AE16"/>
     <mergeCell ref="A4:I4"/>
     <mergeCell ref="G21:G22"/>
     <mergeCell ref="H21:H22"/>
@@ -29539,22 +29575,15 @@
     <mergeCell ref="A21:A24"/>
     <mergeCell ref="A15:F17"/>
     <mergeCell ref="A18:F18"/>
-    <mergeCell ref="K18:N18"/>
-    <mergeCell ref="O18:Q18"/>
-    <mergeCell ref="R18:V18"/>
-    <mergeCell ref="G15:V17"/>
-    <mergeCell ref="W15:AE16"/>
-    <mergeCell ref="AF15:AM17"/>
-    <mergeCell ref="AN15:AO18"/>
-    <mergeCell ref="W17:Y17"/>
-    <mergeCell ref="Z17:AB17"/>
-    <mergeCell ref="AC17:AE17"/>
-    <mergeCell ref="W18:Y18"/>
-    <mergeCell ref="Z18:AB18"/>
-    <mergeCell ref="AC18:AE18"/>
-    <mergeCell ref="AF18:AH18"/>
-    <mergeCell ref="AI18:AK18"/>
-    <mergeCell ref="AL18:AM18"/>
+    <mergeCell ref="P21:P22"/>
+    <mergeCell ref="Q21:Q22"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="M21:M22"/>
+    <mergeCell ref="N21:N22"/>
+    <mergeCell ref="O21:O22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>